<commit_message>
JP-981, 982: Support un/assign Machine from/to Folder
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B935D2D5-FB35-44C0-AE26-13B59BD654DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE625AC-DF59-4424-AE36-30E98CA0A59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="941">
   <si>
     <t>Name</t>
   </si>
@@ -973,9 +973,6 @@
     <t>Unsupported operation.</t>
   </si>
   <si>
-    <t>操作はサポートされていません。</t>
-  </si>
-  <si>
     <t>OperationDefaultResult</t>
   </si>
   <si>
@@ -1098,9 +1095,6 @@
   </si>
   <si>
     <t>ProgressStatus</t>
-  </si>
-  <si>
-    <t>Progress status: {0} / {1}.</t>
   </si>
   <si>
     <t>進捗ステータス: {0} / {1}。</t>
@@ -3040,6 +3034,59 @@
     </rPh>
     <rPh sb="13" eb="14">
       <t>か</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AssignUnassignFolderMachineOperationName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign or Unassign Machine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>マシンをフォルダーに割り当てまたは解除</t>
+    <rPh sb="10" eb="11">
+      <t>わ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>あ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>かいじょ</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作はサポートされていません。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progress status: {0} / {1}.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AssignRequired</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign is required.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>割り当ては必須項目です。</t>
+    <rPh sb="0" eb="1">
+      <t>わ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>あ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ひっす</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>こうもく</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3113,8 +3160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C336" totalsRowShown="0">
-  <autoFilter ref="A1:C336" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C338" totalsRowShown="0">
+  <autoFilter ref="A1:C338" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -3387,10 +3434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C336"/>
+  <dimension ref="A1:C338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A229" sqref="A229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -4492,2482 +4539,2504 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>932</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>933</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1" t="s">
-        <v>265</v>
+        <v>933</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>266</v>
+        <v>934</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>267</v>
+        <v>935</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>279</v>
+        <v>936</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C115" s="2" t="s">
+    </row>
+    <row r="117" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="1" t="s">
+      <c r="B117" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>320</v>
+        <v>937</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="54" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B127" s="2" t="s">
+    </row>
+    <row r="129" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="B129" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="1" t="s">
+      <c r="C129" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>405</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>413</v>
+        <v>407</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C163" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A163" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C165" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="B164" s="2" t="s">
+    </row>
+    <row r="166" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A165" s="1" t="s">
+      <c r="C166" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C174" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A175" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>480</v>
-      </c>
+      <c r="B175" s="2"/>
+      <c r="C175" s="2"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>524</v>
+        <v>518</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>519</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C194" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B193" s="2" t="s">
+    </row>
+    <row r="195" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="B195" s="2" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A194" s="1" t="s">
+      <c r="C195" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A195" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C204" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="B203" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B204" s="2"/>
-      <c r="C204" s="2"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A205" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>567</v>
-      </c>
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
     </row>
     <row r="206" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="C207" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="B206" s="2" t="s">
+    </row>
+    <row r="208" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="B208" s="2" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A207" s="1" t="s">
+      <c r="C208" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A208" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C211" s="2" t="s">
         <v>580</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A212" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="1" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="1" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="1" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="1" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1" t="s">
-        <v>634</v>
+        <v>938</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>635</v>
+        <v>939</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>636</v>
+        <v>940</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="1" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A234" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A235" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C235" s="2" t="s">
         <v>646</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A234" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>650</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A235" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="1" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="1" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="1" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="1" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="1" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>732</v>
+        <v>724</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A262" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="1" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A264" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B264" s="2" t="s">
-        <v>737</v>
-      </c>
-      <c r="C264" s="2" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="1" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="1" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>747</v>
+        <v>739</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A268" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A270" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="B270" s="2" t="s">
-        <v>752</v>
-      </c>
-      <c r="C270" s="2" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>746</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="1" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>758</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>759</v>
+        <v>750</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="1" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="1" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>764</v>
-      </c>
-      <c r="C274" s="2" t="s">
-        <v>765</v>
+        <v>756</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="B275" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="C275" s="2" t="s">
-        <v>768</v>
+        <v>758</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="1" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>771</v>
+        <v>763</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A277" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A280" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="C280" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="B278" s="2" t="s">
-        <v>773</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A279" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="B279" s="2" t="s">
-        <v>776</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B280" s="2"/>
-      <c r="C280" s="2"/>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="1" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A282" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="B282" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="C282" s="2" t="s">
-        <v>783</v>
-      </c>
+      <c r="B282" s="2"/>
+      <c r="C282" s="2"/>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="1" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="1" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="1" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B290" s="2"/>
-      <c r="C290" s="2"/>
+      <c r="A290" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A292" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="B292" s="2" t="s">
-        <v>809</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>810</v>
-      </c>
+      <c r="B292" s="2"/>
+      <c r="C292" s="2"/>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="1" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="1" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="1" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="1" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="1" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="1" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A304" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A305" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C305" s="2" t="s">
         <v>841</v>
       </c>
-      <c r="B303" s="2" t="s">
+    </row>
+    <row r="306" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A306" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="C303" s="2" t="s">
+      <c r="B306" s="2" t="s">
         <v>843</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A304" s="1" t="s">
+      <c r="C306" s="2" t="s">
         <v>844</v>
-      </c>
-      <c r="B304" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C304" s="2" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A306" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="B306" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="C306" s="1" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A307" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="B307" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="C307" s="1" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="1" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="1" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="B310" s="2" t="s">
-        <v>860</v>
-      </c>
-      <c r="C310" s="2" t="s">
-        <v>861</v>
+        <v>851</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="1" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="1" t="s">
-        <v>865</v>
-      </c>
-      <c r="B312" s="1" t="s">
-        <v>866</v>
-      </c>
-      <c r="C312" s="1" t="s">
-        <v>867</v>
+        <v>857</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>859</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="1" t="s">
-        <v>868</v>
-      </c>
-      <c r="B313" s="2" t="s">
-        <v>869</v>
-      </c>
-      <c r="C313" s="2" t="s">
-        <v>870</v>
+        <v>860</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>862</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="1" t="s">
-        <v>871</v>
-      </c>
-      <c r="B314" s="2" t="s">
-        <v>824</v>
-      </c>
-      <c r="C314" s="2" t="s">
-        <v>825</v>
+        <v>863</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="B315" s="1" t="s">
-        <v>873</v>
+        <v>866</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>867</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="1" t="s">
-        <v>875</v>
-      </c>
-      <c r="B316" s="1" t="s">
-        <v>876</v>
+        <v>869</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>822</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>877</v>
+        <v>823</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="1" t="s">
-        <v>878</v>
-      </c>
-      <c r="B317" s="2" t="s">
-        <v>879</v>
+        <v>870</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>871</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A319" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A320" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="C320" s="2" t="s">
         <v>881</v>
       </c>
-      <c r="B318" s="2" t="s">
+    </row>
+    <row r="321" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A321" s="1" t="s">
         <v>882</v>
       </c>
-      <c r="C318" s="2" t="s">
+      <c r="B321" s="2" t="s">
         <v>883</v>
       </c>
-    </row>
-    <row r="319" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A319" s="1" t="s">
+      <c r="C321" s="2" t="s">
         <v>884</v>
-      </c>
-      <c r="B319" s="2" t="s">
-        <v>885</v>
-      </c>
-      <c r="C319" s="2" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A321" s="1" t="s">
-        <v>887</v>
-      </c>
-      <c r="B321" s="2" t="s">
-        <v>888</v>
-      </c>
-      <c r="C321" s="2" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A322" s="1" t="s">
-        <v>890</v>
-      </c>
-      <c r="B322" s="2" t="s">
-        <v>891</v>
-      </c>
-      <c r="C322" s="2" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="1" t="s">
-        <v>893</v>
-      </c>
-      <c r="B323" s="1" t="s">
-        <v>894</v>
-      </c>
-      <c r="C323" s="1" t="s">
-        <v>895</v>
+        <v>885</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="1" t="s">
-        <v>896</v>
-      </c>
-      <c r="B324" s="1" t="s">
-        <v>897</v>
-      </c>
-      <c r="C324" s="1" t="s">
-        <v>898</v>
+        <v>888</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="1" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="1" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" s="1" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="1" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="1" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="1" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="1" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="1" t="s">
-        <v>923</v>
-      </c>
-      <c r="B333" s="2" t="s">
-        <v>924</v>
-      </c>
-      <c r="C333" s="2" t="s">
-        <v>925</v>
+        <v>915</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="B334" s="2" t="s">
-        <v>927</v>
-      </c>
-      <c r="C334" s="2" t="s">
-        <v>928</v>
+        <v>918</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A335" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A338" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="C338" s="1" t="s">
         <v>929</v>
-      </c>
-      <c r="B336" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="C336" s="1" t="s">
-        <v>931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issues with Get Triggers and Assign Machines
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE625AC-DF59-4424-AE36-30E98CA0A59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139FF437-DFAA-4F94-9673-CC2CA4732822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="2" r:id="rId1"/>
@@ -3046,19 +3046,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>マシンをフォルダーに割り当てまたは解除</t>
-    <rPh sb="10" eb="11">
-      <t>わ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>あ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>かいじょ</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>操作はサポートされていません。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3087,6 +3074,19 @@
     </rPh>
     <rPh sb="7" eb="9">
       <t>こうもく</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>マシンを割り当てまたは解除</t>
+    <rPh sb="4" eb="5">
+      <t>わ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>あ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>かいじょ</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3436,18 +3436,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="A229" sqref="A229"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="50.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="84.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>73</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>83</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>86</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>89</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>92</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>98</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>101</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>107</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>110</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>113</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>116</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>119</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>122</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>125</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" ht="57.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>128</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>131</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>134</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>140</v>
       </c>
@@ -3986,11 +3986,11 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>143</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>146</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>149</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>152</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>155</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>158</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>161</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>164</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>167</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>170</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>173</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>176</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
         <v>179</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
         <v>182</v>
       </c>
@@ -4144,11 +4144,11 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
         <v>185</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
         <v>186</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>189</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>190</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>191</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>192</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>193</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>194</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>53</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>195</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>196</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>197</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>198</v>
       </c>
@@ -4291,11 +4291,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>199</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>202</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>205</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>208</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
         <v>211</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>214</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>217</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>220</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>223</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
         <v>226</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
         <v>229</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>232</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
         <v>235</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
         <v>238</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
         <v>241</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
         <v>244</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>247</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
         <v>250</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
         <v>253</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
         <v>256</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
         <v>259</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
         <v>262</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
         <v>930</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
         <v>933</v>
       </c>
@@ -4556,10 +4556,10 @@
         <v>934</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
         <v>265</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
         <v>268</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
         <v>271</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
         <v>274</v>
       </c>
@@ -4600,10 +4600,10 @@
         <v>275</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
         <v>276</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
         <v>279</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
         <v>282</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
         <v>285</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
         <v>288</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
         <v>291</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
         <v>294</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
         <v>297</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
         <v>300</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
         <v>303</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
         <v>306</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
         <v>309</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A120" s="1" t="s">
         <v>312</v>
       </c>
@@ -4746,18 +4746,18 @@
         <v>314</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A121" s="1" t="s">
         <v>315</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
         <v>320</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
         <v>323</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
         <v>326</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A126" s="1" t="s">
         <v>329</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A127" s="1" t="s">
         <v>332</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A128" s="1" t="s">
         <v>335</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
         <v>338</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
         <v>341</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
         <v>344</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
         <v>347</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
         <v>350</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
         <v>353</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A135" s="1" t="s">
         <v>356</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A136" s="1" t="s">
         <v>359</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A137" s="1" t="s">
         <v>362</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A138" s="1" t="s">
         <v>365</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A139" s="1" t="s">
         <v>368</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A140" s="1" t="s">
         <v>371</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
         <v>374</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A142" s="1" t="s">
         <v>377</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A143" s="1" t="s">
         <v>380</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A144" s="1" t="s">
         <v>383</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="1" t="s">
         <v>386</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A146" s="1" t="s">
         <v>389</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A147" s="1" t="s">
         <v>392</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A148" s="1" t="s">
         <v>395</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A149" s="1" t="s">
         <v>398</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A150" s="1" t="s">
         <v>401</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A151" s="1" t="s">
         <v>404</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A152" s="1" t="s">
         <v>407</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A153" s="1" t="s">
         <v>410</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A154" s="1" t="s">
         <v>413</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A155" s="1" t="s">
         <v>416</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="1" t="s">
         <v>419</v>
       </c>
@@ -5142,7 +5142,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A157" s="1" t="s">
         <v>422</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="1" t="s">
         <v>425</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A159" s="1" t="s">
         <v>428</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A160" s="1" t="s">
         <v>431</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A161" s="1" t="s">
         <v>434</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A162" s="1" t="s">
         <v>437</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A163" s="1" t="s">
         <v>440</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A164" s="1" t="s">
         <v>443</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A165" s="1" t="s">
         <v>446</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.4">
       <c r="A166" s="1" t="s">
         <v>449</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A167" s="1" t="s">
         <v>452</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A168" s="1" t="s">
         <v>455</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A169" s="1" t="s">
         <v>458</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A170" s="1" t="s">
         <v>461</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A171" s="1" t="s">
         <v>464</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A172" s="1" t="s">
         <v>467</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A173" s="1" t="s">
         <v>470</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A174" s="1" t="s">
         <v>473</v>
       </c>
@@ -5340,11 +5340,11 @@
         <v>475</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A176" s="1" t="s">
         <v>476</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A177" s="1" t="s">
         <v>479</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A178" s="1" t="s">
         <v>482</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A179" s="1" t="s">
         <v>485</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A180" s="1" t="s">
         <v>488</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A181" s="1" t="s">
         <v>491</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A182" s="1" t="s">
         <v>494</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A183" s="1" t="s">
         <v>497</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
         <v>500</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A185" s="1" t="s">
         <v>503</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A186" s="1" t="s">
         <v>506</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A187" s="1" t="s">
         <v>509</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A188" s="1" t="s">
         <v>512</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A189" s="1" t="s">
         <v>515</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A190" s="1" t="s">
         <v>518</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
         <v>521</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
         <v>524</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
         <v>527</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
         <v>530</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A195" s="1" t="s">
         <v>533</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
         <v>536</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
         <v>539</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
         <v>542</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
         <v>545</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A200" s="1" t="s">
         <v>548</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
         <v>551</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
         <v>554</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
         <v>557</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
         <v>560</v>
       </c>
@@ -5663,11 +5663,11 @@
         <v>562</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
     </row>
-    <row r="206" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
         <v>563</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
         <v>566</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A208" s="1" t="s">
         <v>569</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
         <v>572</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
         <v>575</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
         <v>578</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
         <v>581</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
         <v>584</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A215" s="1" t="s">
         <v>587</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
         <v>590</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
         <v>593</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
         <v>596</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
         <v>599</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
         <v>602</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A221" s="1" t="s">
         <v>605</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A222" s="1" t="s">
         <v>608</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A223" s="1" t="s">
         <v>611</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A224" s="1" t="s">
         <v>614</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A225" s="1" t="s">
         <v>617</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A226" s="1" t="s">
         <v>620</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A227" s="1" t="s">
         <v>623</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A228" s="1" t="s">
         <v>626</v>
       </c>
@@ -5909,18 +5909,18 @@
         <v>628</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A229" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>938</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="C229" s="2" t="s">
         <v>939</v>
       </c>
-      <c r="C229" s="2" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="230" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A230" s="1" t="s">
         <v>629</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A231" s="1" t="s">
         <v>632</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A232" s="1" t="s">
         <v>635</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A233" s="1" t="s">
         <v>638</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A234" s="1" t="s">
         <v>641</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A235" s="1" t="s">
         <v>644</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A236" s="1" t="s">
         <v>647</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A237" s="1" t="s">
         <v>650</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A238" s="1" t="s">
         <v>653</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A239" s="1" t="s">
         <v>656</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A240" s="1" t="s">
         <v>659</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A241" s="1" t="s">
         <v>662</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A242" s="1" t="s">
         <v>665</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A243" s="1" t="s">
         <v>668</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A244" s="1" t="s">
         <v>671</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A245" s="1" t="s">
         <v>674</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A246" s="1" t="s">
         <v>677</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A247" s="1" t="s">
         <v>680</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A248" s="1" t="s">
         <v>683</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A249" s="1" t="s">
         <v>686</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A250" s="1" t="s">
         <v>689</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A251" s="1" t="s">
         <v>692</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A252" s="1" t="s">
         <v>695</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A253" s="1" t="s">
         <v>698</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A254" s="1" t="s">
         <v>701</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A255" s="1" t="s">
         <v>704</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A256" s="1" t="s">
         <v>707</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A257" s="1" t="s">
         <v>710</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A258" s="1" t="s">
         <v>713</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A259" s="1" t="s">
         <v>716</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A260" s="1" t="s">
         <v>719</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A261" s="1" t="s">
         <v>722</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A262" s="1" t="s">
         <v>725</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A263" s="1" t="s">
         <v>728</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A265" s="1" t="s">
         <v>731</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A266" s="1" t="s">
         <v>734</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="267" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A267" s="1" t="s">
         <v>737</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="268" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A268" s="1" t="s">
         <v>740</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A269" s="1" t="s">
         <v>743</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A271" s="1" t="s">
         <v>746</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A272" s="1" t="s">
         <v>749</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A273" s="1" t="s">
         <v>752</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A274" s="1" t="s">
         <v>755</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A275" s="1" t="s">
         <v>758</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A276" s="1" t="s">
         <v>761</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A277" s="1" t="s">
         <v>764</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A278" s="1" t="s">
         <v>767</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A280" s="1" t="s">
         <v>770</v>
       </c>
@@ -6448,7 +6448,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A281" s="1" t="s">
         <v>773</v>
       </c>
@@ -6459,11 +6459,11 @@
         <v>775</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A283" s="1" t="s">
         <v>776</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A284" s="1" t="s">
         <v>779</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A285" s="1" t="s">
         <v>782</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A286" s="1" t="s">
         <v>785</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A287" s="1" t="s">
         <v>788</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A288" s="1" t="s">
         <v>791</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A289" s="1" t="s">
         <v>794</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A290" s="1" t="s">
         <v>797</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A291" s="1" t="s">
         <v>800</v>
       </c>
@@ -6562,11 +6562,11 @@
         <v>802</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A293" s="1" t="s">
         <v>803</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A294" s="1" t="s">
         <v>806</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A295" s="1" t="s">
         <v>809</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A296" s="1" t="s">
         <v>812</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A297" s="1" t="s">
         <v>815</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A298" s="1" t="s">
         <v>818</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A299" s="1" t="s">
         <v>821</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A300" s="1" t="s">
         <v>824</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A301" s="1" t="s">
         <v>827</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A302" s="1" t="s">
         <v>830</v>
       </c>
@@ -6676,7 +6676,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A303" s="1" t="s">
         <v>833</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A304" s="1" t="s">
         <v>836</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A305" s="1" t="s">
         <v>839</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A306" s="1" t="s">
         <v>842</v>
       </c>
@@ -6720,7 +6720,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A308" s="1" t="s">
         <v>845</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A309" s="1" t="s">
         <v>848</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A310" s="1" t="s">
         <v>851</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A311" s="1" t="s">
         <v>854</v>
       </c>
@@ -6764,7 +6764,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A312" s="1" t="s">
         <v>857</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A313" s="1" t="s">
         <v>860</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A314" s="1" t="s">
         <v>863</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A315" s="1" t="s">
         <v>866</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A316" s="1" t="s">
         <v>869</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A317" s="1" t="s">
         <v>870</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="318" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A318" s="1" t="s">
         <v>873</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A319" s="1" t="s">
         <v>876</v>
       </c>
@@ -6852,7 +6852,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A320" s="1" t="s">
         <v>879</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="321" spans="1:3" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A321" s="1" t="s">
         <v>882</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A323" s="1" t="s">
         <v>885</v>
       </c>
@@ -6885,7 +6885,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A324" s="1" t="s">
         <v>888</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A325" s="1" t="s">
         <v>891</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A326" s="1" t="s">
         <v>894</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A327" s="1" t="s">
         <v>897</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A328" s="1" t="s">
         <v>900</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A329" s="1" t="s">
         <v>903</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A330" s="1" t="s">
         <v>906</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A331" s="1" t="s">
         <v>909</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A332" s="1" t="s">
         <v>912</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A333" s="1" t="s">
         <v>915</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A334" s="1" t="s">
         <v>918</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A335" s="1" t="s">
         <v>921</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A336" s="1" t="s">
         <v>924</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A338" s="1" t="s">
         <v>927</v>
       </c>

</xml_diff>

<commit_message>
Fix typo in Translation.xlsx
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139FF437-DFAA-4F94-9673-CC2CA4732822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA27361-3ADC-484E-851C-1A7618A4904B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38140" yWindow="430" windowWidth="37500" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="2" r:id="rId1"/>
@@ -3078,7 +3078,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>マシンを割り当てまたは解除</t>
+    <t>マシンの割り当てまたは解除</t>
     <rPh sb="4" eb="5">
       <t>わ</t>
     </rPh>
@@ -3436,8 +3436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Add OAuth authentication option for Cloud and On-Premises >= 21.4
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA27361-3ADC-484E-851C-1A7618A4904B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4CCEAC-F512-4C4D-AA3E-EBE29AFD5416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38140" yWindow="430" windowWidth="37500" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="950">
   <si>
     <t>Name</t>
   </si>
@@ -3087,6 +3087,42 @@
     </rPh>
     <rPh sb="11" eb="13">
       <t>かいじょ</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormAppIDLabel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormAppSecretLabel</t>
+  </si>
+  <si>
+    <t>App ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>App Secret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>アプリ シークレット</t>
+  </si>
+  <si>
+    <t>アプリ ID</t>
+  </si>
+  <si>
+    <t>FormUseOAuthFlow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use OAuth flow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OAuth フローを使用します。</t>
+    <rPh sb="10" eb="12">
+      <t>ｼﾖｳ</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3160,8 +3196,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C338" totalsRowShown="0">
-  <autoFilter ref="A1:C338" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C341" totalsRowShown="0">
+  <autoFilter ref="A1:C341" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="EN"/>
@@ -3434,7 +3470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C338"/>
+  <dimension ref="A1:C341"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3658,3384 +3694,3418 @@
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>941</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>943</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>946</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>942</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>944</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>945</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>947</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>62</v>
+        <v>948</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>949</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="57.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="75" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="93.75" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="A65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A68" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>72</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
-        <v>53</v>
+        <v>192</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>53</v>
+        <v>192</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>196</v>
+        <v>50</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>197</v>
+        <v>53</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>197</v>
+        <v>53</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>204</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A82" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>207</v>
-      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
-        <v>930</v>
+        <v>256</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>931</v>
+        <v>257</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>932</v>
+        <v>258</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
-        <v>933</v>
+        <v>259</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>934</v>
+        <v>260</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>940</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>268</v>
+        <v>930</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>269</v>
+        <v>931</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>270</v>
+        <v>932</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>271</v>
+        <v>933</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>272</v>
+        <v>934</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>273</v>
+        <v>940</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>935</v>
+        <v>267</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>284</v>
+        <v>935</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A120" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A121" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>936</v>
+        <v>307</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A122" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>324</v>
+        <v>936</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A126" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A127" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A128" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A135" s="1" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A136" s="1" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A137" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A138" s="1" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A139" s="1" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A140" s="1" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A142" s="1" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A143" s="1" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A144" s="1" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="1" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A146" s="1" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A147" s="1" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A148" s="1" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A149" s="1" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A150" s="1" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A151" s="1" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A152" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>408</v>
+        <v>398</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>399</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A153" s="1" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A154" s="1" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A155" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>417</v>
+        <v>407</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="1" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A157" s="1" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="1" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A159" s="1" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A160" s="1" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A161" s="1" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A162" s="1" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A163" s="1" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A164" s="1" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A165" s="1" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="75" x14ac:dyDescent="0.4">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A166" s="1" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A167" s="1" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A168" s="1" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A169" s="1" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A170" s="1" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A171" s="1" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A172" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A173" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A174" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A175" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B175" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C175" s="2" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A173" s="1" t="s">
+    <row r="176" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A176" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B176" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A174" s="1" t="s">
+    <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A177" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B177" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C177" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A176" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A177" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A178" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>484</v>
-      </c>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
     </row>
     <row r="179" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A179" s="1" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A180" s="1" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A181" s="1" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A182" s="1" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A183" s="1" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A185" s="1" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A186" s="1" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A187" s="1" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A188" s="1" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A189" s="1" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A190" s="1" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>522</v>
+        <v>512</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>513</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>525</v>
+        <v>515</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>516</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>528</v>
+        <v>518</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>519</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>531</v>
+        <v>521</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>522</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A195" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>534</v>
+        <v>524</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>537</v>
+        <v>527</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>528</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A200" s="1" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B205" s="2"/>
-      <c r="C205" s="2"/>
+      <c r="A205" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="206" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A208" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>571</v>
-      </c>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B208" s="2"/>
+      <c r="C208" s="2"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>580</v>
+        <v>571</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A212" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A215" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A221" s="1" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A222" s="1" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A223" s="1" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A224" s="1" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A225" s="1" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A226" s="1" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A227" s="1" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A228" s="1" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A229" s="1" t="s">
-        <v>937</v>
+        <v>620</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>938</v>
+        <v>621</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>939</v>
+        <v>622</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A230" s="1" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A231" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A232" s="1" t="s">
-        <v>635</v>
+        <v>937</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>636</v>
+        <v>938</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>637</v>
+        <v>939</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A233" s="1" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A234" s="1" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A235" s="1" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A236" s="1" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A237" s="1" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A238" s="1" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A239" s="1" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A240" s="1" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A241" s="1" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A242" s="1" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A243" s="1" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A244" s="1" t="s">
-        <v>671</v>
+        <v>662</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A245" s="1" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.4">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A246" s="1" t="s">
-        <v>677</v>
+        <v>668</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>678</v>
+        <v>669</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>679</v>
+        <v>670</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A247" s="1" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>681</v>
+        <v>672</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>682</v>
+        <v>673</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A248" s="1" t="s">
-        <v>683</v>
+        <v>674</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>684</v>
+        <v>675</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>685</v>
+        <v>676</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A249" s="1" t="s">
-        <v>686</v>
+        <v>677</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>687</v>
+        <v>678</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>688</v>
+        <v>679</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A250" s="1" t="s">
-        <v>689</v>
+        <v>680</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>690</v>
+        <v>681</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>691</v>
+        <v>682</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A251" s="1" t="s">
-        <v>692</v>
+        <v>683</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>693</v>
+        <v>684</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>694</v>
+        <v>685</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A252" s="1" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>696</v>
+        <v>687</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A253" s="1" t="s">
-        <v>698</v>
+        <v>689</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>700</v>
+        <v>691</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A254" s="1" t="s">
-        <v>701</v>
+        <v>692</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>702</v>
+        <v>693</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A255" s="1" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>705</v>
+        <v>696</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A256" s="1" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>708</v>
+        <v>699</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A257" s="1" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A258" s="1" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A259" s="1" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A260" s="1" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A261" s="1" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A262" s="1" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A263" s="1" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>730</v>
+        <v>721</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A264" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A265" s="1" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A266" s="1" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A267" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>738</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A268" s="1" t="s">
-        <v>740</v>
+        <v>731</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>741</v>
+        <v>732</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>742</v>
+        <v>733</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A269" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A270" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A271" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A272" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="B269" s="2" t="s">
+      <c r="B272" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="C269" s="2" t="s">
+      <c r="C272" s="2" t="s">
         <v>745</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A271" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="B271" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A272" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="B272" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="C272" s="2" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A273" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="C273" s="1" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A274" s="1" t="s">
-        <v>755</v>
+        <v>746</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="C274" s="1" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.4">
+        <v>747</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A275" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="B275" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>760</v>
+        <v>749</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A276" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="B276" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="C276" s="2" t="s">
-        <v>763</v>
+        <v>752</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A277" s="1" t="s">
-        <v>764</v>
+        <v>755</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="C277" s="2" t="s">
-        <v>766</v>
+        <v>756</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A278" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="B278" s="2" t="s">
-        <v>768</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>769</v>
+        <v>758</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A279" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A280" s="1" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A281" s="1" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B282" s="2"/>
-      <c r="C282" s="2"/>
+        <v>769</v>
+      </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A283" s="1" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A284" s="1" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A285" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="B285" s="2" t="s">
-        <v>783</v>
-      </c>
-      <c r="C285" s="2" t="s">
-        <v>784</v>
-      </c>
+      <c r="B285" s="2"/>
+      <c r="C285" s="2"/>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A286" s="1" t="s">
-        <v>785</v>
+        <v>776</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A287" s="1" t="s">
-        <v>788</v>
+        <v>779</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>790</v>
+        <v>781</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A288" s="1" t="s">
-        <v>791</v>
+        <v>782</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>792</v>
+        <v>783</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>793</v>
+        <v>784</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A289" s="1" t="s">
-        <v>794</v>
+        <v>785</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>795</v>
+        <v>786</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>796</v>
+        <v>787</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A290" s="1" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A291" s="1" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B292" s="2"/>
-      <c r="C292" s="2"/>
+      <c r="A292" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A293" s="1" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A294" s="1" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A295" s="1" t="s">
-        <v>809</v>
-      </c>
-      <c r="B295" s="2" t="s">
-        <v>810</v>
-      </c>
-      <c r="C295" s="2" t="s">
-        <v>811</v>
-      </c>
+      <c r="B295" s="2"/>
+      <c r="C295" s="2"/>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A296" s="1" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A297" s="1" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>816</v>
+        <v>807</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A298" s="1" t="s">
-        <v>818</v>
+        <v>809</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A299" s="1" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A300" s="1" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>826</v>
+        <v>817</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A301" s="1" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A302" s="1" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A303" s="1" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>834</v>
+        <v>825</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A304" s="1" t="s">
-        <v>836</v>
+        <v>827</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A305" s="1" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A306" s="1" t="s">
-        <v>842</v>
+        <v>833</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>844</v>
+        <v>835</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A307" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A308" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="B308" s="1" t="s">
-        <v>846</v>
-      </c>
-      <c r="C308" s="1" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.4">
+        <v>839</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A309" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="B309" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="C309" s="1" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A310" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="B310" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="C310" s="1" t="s">
-        <v>853</v>
+        <v>842</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A311" s="1" t="s">
-        <v>854</v>
+        <v>845</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>856</v>
+        <v>847</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A312" s="1" t="s">
-        <v>857</v>
-      </c>
-      <c r="B312" s="2" t="s">
-        <v>858</v>
-      </c>
-      <c r="C312" s="2" t="s">
-        <v>859</v>
+        <v>848</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A313" s="1" t="s">
-        <v>860</v>
+        <v>851</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>861</v>
+        <v>852</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>862</v>
+        <v>853</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A314" s="1" t="s">
-        <v>863</v>
+        <v>854</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>864</v>
+        <v>855</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>865</v>
+        <v>856</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A315" s="1" t="s">
-        <v>866</v>
+        <v>857</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>867</v>
+        <v>858</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>868</v>
+        <v>859</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A316" s="1" t="s">
-        <v>869</v>
-      </c>
-      <c r="B316" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>823</v>
+        <v>860</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>862</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A317" s="1" t="s">
-        <v>870</v>
+        <v>863</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>871</v>
-      </c>
-      <c r="C317" s="2" t="s">
-        <v>872</v>
+        <v>864</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A318" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="B318" s="1" t="s">
-        <v>874</v>
+        <v>866</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>867</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>875</v>
+        <v>868</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A319" s="1" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>877</v>
+        <v>822</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>878</v>
+        <v>823</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A320" s="1" t="s">
-        <v>879</v>
-      </c>
-      <c r="B320" s="2" t="s">
-        <v>880</v>
+        <v>870</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>871</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="321" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A321" s="1" t="s">
-        <v>882</v>
-      </c>
-      <c r="B321" s="2" t="s">
-        <v>883</v>
+        <v>873</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>874</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>884</v>
+        <v>875</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A322" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A323" s="1" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.4">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A324" s="1" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A325" s="1" t="s">
-        <v>891</v>
-      </c>
-      <c r="B325" s="1" t="s">
-        <v>892</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>893</v>
+        <v>884</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A326" s="1" t="s">
-        <v>894</v>
-      </c>
-      <c r="B326" s="1" t="s">
-        <v>895</v>
-      </c>
-      <c r="C326" s="1" t="s">
-        <v>896</v>
+        <v>885</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A327" s="1" t="s">
-        <v>897</v>
-      </c>
-      <c r="B327" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="C327" s="1" t="s">
-        <v>899</v>
+        <v>888</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A328" s="1" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A329" s="1" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>904</v>
+        <v>895</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>905</v>
+        <v>896</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A330" s="1" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>908</v>
+        <v>899</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A331" s="1" t="s">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>910</v>
+        <v>901</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>911</v>
+        <v>902</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A332" s="1" t="s">
-        <v>912</v>
+        <v>903</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>913</v>
+        <v>904</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>914</v>
+        <v>905</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A333" s="1" t="s">
-        <v>915</v>
+        <v>906</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A334" s="1" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>919</v>
+        <v>910</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A335" s="1" t="s">
-        <v>921</v>
-      </c>
-      <c r="B335" s="2" t="s">
-        <v>922</v>
-      </c>
-      <c r="C335" s="2" t="s">
-        <v>923</v>
+        <v>912</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>914</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A336" s="1" t="s">
-        <v>924</v>
-      </c>
-      <c r="B336" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="C336" s="2" t="s">
-        <v>926</v>
+        <v>915</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A337" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A338" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A339" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A341" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="B338" s="1" t="s">
+      <c r="B341" s="1" t="s">
         <v>928</v>
       </c>
-      <c r="C338" s="1" t="s">
+      <c r="C341" s="1" t="s">
         <v>929</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Link Asset to multiple Folders
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B601C178-C44F-4D1E-B7CC-938BC611395B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3470926F-E156-486E-B328-A5D5387E2BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="690" windowWidth="28800" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="2250" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="961">
   <si>
     <t>Name</t>
   </si>
@@ -3153,6 +3153,43 @@
   </si>
   <si>
     <t>Update to Specific Package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LinkOrUnlinkNotSpecified</t>
+  </si>
+  <si>
+    <t>Link or Unlink not specified.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>リンクを作成するか削除するかが指定されていません。</t>
+    <rPh sb="4" eb="6">
+      <t>ｻｸｾｲ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ｻｸｼﾞｮ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ｼﾃｲ</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LinkOrUnlinkOperationName</t>
+  </si>
+  <si>
+    <t>Link or Unlink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>リンクを作成または削除</t>
+    <rPh sb="4" eb="6">
+      <t>ｻｸｾｲ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ｻｸｼﾞｮ</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3504,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
-      <selection activeCell="B314" sqref="B314"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5156,1991 +5193,2005 @@
     </row>
     <row r="150" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A150" s="1" t="s">
-        <v>152</v>
+        <v>955</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>153</v>
+        <v>956</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>154</v>
+        <v>957</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A151" s="1" t="s">
-        <v>563</v>
+        <v>958</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>564</v>
+        <v>959</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>565</v>
+        <v>960</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A152" s="1" t="s">
-        <v>578</v>
+        <v>152</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>579</v>
+        <v>153</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>580</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A153" s="1" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A154" s="1" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>567</v>
+        <v>579</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>568</v>
+        <v>580</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A155" s="1" t="s">
-        <v>190</v>
+        <v>572</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>190</v>
+        <v>573</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>69</v>
+        <v>574</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="1" t="s">
-        <v>268</v>
+        <v>566</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>269</v>
+        <v>567</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>270</v>
+        <v>568</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A157" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>853</v>
+        <v>190</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="1" t="s">
-        <v>467</v>
+        <v>268</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>468</v>
+        <v>269</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>469</v>
+        <v>270</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A159" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>634</v>
+        <v>851</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A160" s="1" t="s">
-        <v>250</v>
+        <v>467</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>251</v>
+        <v>468</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A161" s="1" t="s">
-        <v>473</v>
+        <v>632</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>474</v>
+        <v>633</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>475</v>
+        <v>634</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A162" s="1" t="s">
-        <v>647</v>
+        <v>250</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>648</v>
+        <v>251</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A163" s="1" t="s">
-        <v>623</v>
+        <v>473</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>624</v>
+        <v>474</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>625</v>
+        <v>475</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A164" s="1" t="s">
-        <v>800</v>
+        <v>647</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>801</v>
+        <v>648</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>802</v>
+        <v>649</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A165" s="1" t="s">
-        <v>707</v>
+        <v>623</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>708</v>
+        <v>624</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>709</v>
+        <v>625</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A166" s="1" t="s">
-        <v>870</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>871</v>
+        <v>800</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>801</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>872</v>
+        <v>802</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A167" s="1" t="s">
-        <v>656</v>
+        <v>707</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>657</v>
+        <v>708</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>658</v>
+        <v>709</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A168" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>660</v>
+        <v>870</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>871</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>661</v>
+        <v>872</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A169" s="1" t="s">
-        <v>560</v>
+        <v>656</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>561</v>
+        <v>657</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>562</v>
+        <v>658</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A170" s="1" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A171" s="1" t="s">
-        <v>689</v>
+        <v>560</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>690</v>
+        <v>561</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>691</v>
+        <v>562</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A172" s="1" t="s">
-        <v>885</v>
+        <v>668</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>886</v>
+        <v>669</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>887</v>
+        <v>670</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A173" s="1" t="s">
-        <v>698</v>
+        <v>689</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>700</v>
+        <v>691</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A174" s="1" t="s">
-        <v>716</v>
+        <v>885</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>717</v>
+        <v>886</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A175" s="1" t="s">
-        <v>470</v>
+        <v>698</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>471</v>
+        <v>699</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>472</v>
+        <v>700</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A176" s="1" t="s">
-        <v>593</v>
+        <v>716</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>594</v>
+        <v>717</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>595</v>
+        <v>718</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A177" s="1" t="s">
-        <v>641</v>
+        <v>470</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>642</v>
+        <v>471</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>643</v>
+        <v>472</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A178" s="1" t="s">
-        <v>434</v>
+        <v>593</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>435</v>
+        <v>594</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>436</v>
+        <v>595</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A179" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A180" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A181" s="1" t="s">
-        <v>440</v>
+        <v>644</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>441</v>
+        <v>645</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>442</v>
+        <v>646</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A182" s="1" t="s">
-        <v>350</v>
+        <v>437</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>351</v>
+        <v>438</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>352</v>
+        <v>439</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A183" s="1" t="s">
-        <v>767</v>
+        <v>440</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>768</v>
+        <v>441</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>769</v>
+        <v>442</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
-        <v>599</v>
+        <v>350</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>600</v>
+        <v>351</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>601</v>
+        <v>352</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A185" s="1" t="s">
-        <v>575</v>
+        <v>767</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>576</v>
+        <v>768</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>577</v>
+        <v>769</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A186" s="1" t="s">
-        <v>389</v>
+        <v>599</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>390</v>
+        <v>600</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>391</v>
+        <v>601</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A187" s="1" t="s">
-        <v>743</v>
+        <v>575</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>744</v>
+        <v>576</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>745</v>
+        <v>577</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A188" s="1" t="s">
-        <v>794</v>
+        <v>389</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>795</v>
+        <v>390</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>796</v>
+        <v>391</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A189" s="1" t="s">
-        <v>857</v>
+        <v>743</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>858</v>
+        <v>744</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>859</v>
+        <v>745</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A190" s="1" t="s">
-        <v>554</v>
+        <v>794</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>555</v>
+        <v>795</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>556</v>
+        <v>796</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
-        <v>773</v>
+        <v>857</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>774</v>
+        <v>858</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>775</v>
+        <v>859</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
-        <v>924</v>
+        <v>554</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>925</v>
+        <v>555</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>926</v>
+        <v>556</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
-        <v>503</v>
+        <v>773</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>504</v>
+        <v>774</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>505</v>
+        <v>775</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
-        <v>347</v>
+        <v>924</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>348</v>
+        <v>925</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>349</v>
+        <v>926</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A195" s="1" t="s">
-        <v>818</v>
+        <v>503</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>819</v>
+        <v>504</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>820</v>
+        <v>505</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
-        <v>512</v>
+        <v>347</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>513</v>
+        <v>348</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>514</v>
+        <v>349</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
-        <v>614</v>
+        <v>818</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>615</v>
+        <v>819</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>616</v>
+        <v>820</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
-        <v>332</v>
+        <v>512</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>333</v>
+        <v>513</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>334</v>
+        <v>514</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
-        <v>329</v>
+        <v>614</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>330</v>
+        <v>615</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>331</v>
+        <v>616</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A200" s="1" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>281</v>
+        <v>334</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
-        <v>377</v>
+        <v>329</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>378</v>
+        <v>330</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>379</v>
+        <v>331</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
-        <v>620</v>
+        <v>377</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>621</v>
+        <v>378</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>622</v>
+        <v>379</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A205" s="1" t="s">
-        <v>161</v>
+        <v>620</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>162</v>
+        <v>621</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>163</v>
+        <v>622</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
-        <v>194</v>
+        <v>282</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>51</v>
+        <v>284</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
-        <v>497</v>
+        <v>161</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>498</v>
+        <v>162</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>499</v>
+        <v>163</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A208" s="1" t="s">
-        <v>392</v>
+        <v>194</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>393</v>
+        <v>50</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>394</v>
+        <v>51</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
-        <v>380</v>
+        <v>497</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>381</v>
+        <v>498</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>382</v>
+        <v>499</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
-        <v>740</v>
+        <v>380</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>741</v>
+        <v>381</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>742</v>
+        <v>382</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A212" s="1" t="s">
-        <v>734</v>
+        <v>386</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>735</v>
+        <v>387</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A215" s="1" t="s">
-        <v>833</v>
+        <v>737</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>834</v>
+        <v>738</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>835</v>
+        <v>739</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
-        <v>173</v>
+        <v>731</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>174</v>
+        <v>732</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>175</v>
+        <v>733</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
-        <v>827</v>
+        <v>833</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>828</v>
+        <v>834</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>829</v>
+        <v>835</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
-        <v>821</v>
+        <v>827</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>822</v>
+        <v>828</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>823</v>
+        <v>829</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
-        <v>809</v>
+        <v>182</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>810</v>
+        <v>183</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>811</v>
+        <v>184</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A221" s="1" t="s">
-        <v>803</v>
+        <v>821</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>804</v>
+        <v>822</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>805</v>
+        <v>823</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A222" s="1" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A223" s="1" t="s">
-        <v>196</v>
+        <v>803</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>196</v>
+        <v>804</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>88</v>
+        <v>805</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A224" s="1" t="s">
-        <v>806</v>
+        <v>812</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>952</v>
+        <v>813</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>953</v>
+        <v>814</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A225" s="1" t="s">
-        <v>806</v>
+        <v>196</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>807</v>
+        <v>196</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>808</v>
+        <v>88</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A226" s="1" t="s">
-        <v>312</v>
+        <v>806</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>313</v>
+        <v>952</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>314</v>
+        <v>953</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A227" s="1" t="s">
-        <v>461</v>
+        <v>806</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>462</v>
+        <v>807</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>463</v>
+        <v>808</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A228" s="1" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A229" s="1" t="s">
-        <v>431</v>
+        <v>461</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>432</v>
+        <v>462</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>433</v>
+        <v>463</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A230" s="1" t="s">
-        <v>158</v>
+        <v>335</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>159</v>
+        <v>336</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>160</v>
+        <v>337</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A231" s="1" t="s">
-        <v>341</v>
+        <v>431</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>342</v>
+        <v>432</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>343</v>
+        <v>433</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A232" s="1" t="s">
-        <v>533</v>
+        <v>158</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>534</v>
+        <v>159</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>535</v>
+        <v>160</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A233" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A234" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A235" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B235" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="C235" s="2" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A234" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A235" s="1" t="s">
-        <v>791</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>792</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A236" s="1" t="s">
-        <v>779</v>
+        <v>193</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>780</v>
+        <v>193</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>781</v>
+        <v>78</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A237" s="1" t="s">
-        <v>713</v>
+        <v>791</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>714</v>
+        <v>792</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>715</v>
+        <v>793</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A238" s="1" t="s">
-        <v>710</v>
+        <v>779</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>711</v>
+        <v>780</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>712</v>
+        <v>781</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A239" s="1" t="s">
-        <v>797</v>
+        <v>713</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>798</v>
+        <v>714</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>799</v>
+        <v>715</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A240" s="1" t="s">
-        <v>776</v>
+        <v>710</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>777</v>
+        <v>711</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>778</v>
+        <v>712</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A241" s="1" t="s">
-        <v>782</v>
+        <v>797</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>783</v>
+        <v>798</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>784</v>
+        <v>799</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A242" s="1" t="s">
-        <v>785</v>
+        <v>776</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A243" s="1" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A244" s="1" t="s">
-        <v>315</v>
+        <v>785</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>936</v>
+        <v>786</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>316</v>
+        <v>787</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A245" s="1" t="s">
-        <v>170</v>
+        <v>788</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>171</v>
+        <v>789</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>172</v>
+        <v>790</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A246" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>874</v>
+        <v>315</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>936</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>875</v>
+        <v>316</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A247" s="1" t="s">
-        <v>869</v>
+        <v>170</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>822</v>
+        <v>171</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>823</v>
+        <v>172</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A248" s="1" t="s">
-        <v>863</v>
+        <v>873</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>864</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>865</v>
+        <v>874</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A249" s="1" t="s">
-        <v>665</v>
+        <v>869</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>666</v>
+        <v>822</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>667</v>
+        <v>823</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A250" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="B250" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="C250" s="2" t="s">
-        <v>664</v>
+        <v>863</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A251" s="1" t="s">
-        <v>866</v>
+        <v>665</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>867</v>
+        <v>666</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>868</v>
+        <v>667</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A252" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>862</v>
+        <v>662</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A253" s="1" t="s">
-        <v>854</v>
-      </c>
-      <c r="B253" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>856</v>
+        <v>866</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>868</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A254" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="B254" s="2" t="s">
-        <v>877</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>878</v>
+        <v>860</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>862</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A255" s="1" t="s">
-        <v>879</v>
-      </c>
-      <c r="B255" s="2" t="s">
-        <v>880</v>
-      </c>
-      <c r="C255" s="2" t="s">
-        <v>881</v>
+        <v>854</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A256" s="1" t="s">
-        <v>195</v>
+        <v>876</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>195</v>
+        <v>877</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>85</v>
+        <v>878</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A257" s="1" t="s">
-        <v>761</v>
+        <v>879</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>762</v>
+        <v>880</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>763</v>
+        <v>881</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A258" s="1" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A259" s="1" t="s">
-        <v>509</v>
+        <v>761</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>510</v>
+        <v>762</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A260" s="1" t="s">
-        <v>749</v>
+        <v>149</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>750</v>
+        <v>150</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>751</v>
+        <v>151</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A261" s="1" t="s">
-        <v>551</v>
+        <v>509</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>552</v>
+        <v>510</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.4">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A262" s="1" t="s">
-        <v>548</v>
+        <v>749</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>549</v>
+        <v>750</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>550</v>
+        <v>751</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A263" s="1" t="s">
-        <v>695</v>
+        <v>551</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>696</v>
+        <v>552</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>697</v>
+        <v>553</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A264" s="1" t="s">
-        <v>692</v>
+        <v>548</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>693</v>
+        <v>549</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>694</v>
+        <v>550</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A265" s="1" t="s">
-        <v>557</v>
+        <v>695</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>558</v>
+        <v>696</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>559</v>
+        <v>697</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A266" s="1" t="s">
-        <v>542</v>
+        <v>692</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>543</v>
+        <v>693</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>544</v>
+        <v>694</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A267" s="1" t="s">
-        <v>536</v>
+        <v>557</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>537</v>
+        <v>558</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>538</v>
+        <v>559</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A268" s="1" t="s">
-        <v>191</v>
+        <v>542</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>191</v>
+        <v>543</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>72</v>
+        <v>544</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A269" s="1" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A270" s="1" t="s">
-        <v>500</v>
+        <v>191</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>501</v>
+        <v>191</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>502</v>
+        <v>72</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A271" s="1" t="s">
-        <v>602</v>
+        <v>545</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>603</v>
+        <v>546</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>604</v>
+        <v>547</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A272" s="1" t="s">
-        <v>605</v>
+        <v>500</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>606</v>
+        <v>501</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>607</v>
+        <v>502</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A273" s="1" t="s">
-        <v>770</v>
+        <v>602</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>771</v>
+        <v>603</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>772</v>
+        <v>604</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A274" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A275" s="1" t="s">
-        <v>232</v>
+        <v>770</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>233</v>
+        <v>771</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>234</v>
+        <v>772</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A276" s="1" t="s">
-        <v>368</v>
+        <v>611</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>369</v>
+        <v>612</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>370</v>
+        <v>613</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A277" s="1" t="s">
-        <v>371</v>
+        <v>232</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>372</v>
+        <v>233</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>373</v>
+        <v>234</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A278" s="1" t="s">
-        <v>830</v>
+        <v>368</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>831</v>
+        <v>369</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A279" s="1" t="s">
-        <v>320</v>
+        <v>371</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>321</v>
+        <v>372</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>322</v>
+        <v>373</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A280" s="1" t="s">
-        <v>897</v>
-      </c>
-      <c r="B280" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.4">
+        <v>830</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A281" s="1" t="s">
-        <v>900</v>
-      </c>
-      <c r="B281" s="1" t="s">
-        <v>901</v>
-      </c>
-      <c r="C281" s="1" t="s">
-        <v>902</v>
+        <v>320</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A282" s="1" t="s">
-        <v>912</v>
+        <v>897</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>913</v>
+        <v>898</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>914</v>
+        <v>899</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A283" s="1" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A284" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B284" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C284" s="2" t="s">
-        <v>481</v>
+        <v>912</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>914</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A285" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B285" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C285" s="2" t="s">
-        <v>267</v>
+        <v>903</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>905</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A286" s="1" t="s">
-        <v>906</v>
-      </c>
-      <c r="B286" s="1" t="s">
-        <v>907</v>
-      </c>
-      <c r="C286" s="1" t="s">
-        <v>908</v>
+        <v>479</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A287" s="1" t="s">
-        <v>488</v>
+        <v>265</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>489</v>
+        <v>266</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>490</v>
+        <v>267</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A288" s="1" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A289" s="1" t="s">
-        <v>306</v>
+        <v>488</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>307</v>
+        <v>489</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A290" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B290" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C290" s="2" t="s">
-        <v>296</v>
+        <v>909</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A291" s="1" t="s">
-        <v>179</v>
+        <v>306</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>180</v>
+        <v>307</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.4">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A292" s="1" t="s">
-        <v>918</v>
-      </c>
-      <c r="B292" s="1" t="s">
-        <v>919</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>920</v>
+        <v>294</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A293" s="1" t="s">
-        <v>888</v>
+        <v>179</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>889</v>
+        <v>180</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>890</v>
+        <v>181</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A294" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="B294" s="2" t="s">
-        <v>705</v>
-      </c>
-      <c r="C294" s="2" t="s">
-        <v>706</v>
+        <v>918</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A295" s="1" t="s">
-        <v>701</v>
+        <v>888</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>702</v>
+        <v>889</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>703</v>
+        <v>890</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A296" s="1" t="s">
-        <v>921</v>
+        <v>704</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>922</v>
+        <v>705</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>923</v>
+        <v>706</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A297" s="1" t="s">
-        <v>891</v>
-      </c>
-      <c r="B297" s="1" t="s">
-        <v>892</v>
-      </c>
-      <c r="C297" s="1" t="s">
-        <v>893</v>
+        <v>701</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A298" s="1" t="s">
-        <v>915</v>
-      </c>
-      <c r="B298" s="1" t="s">
-        <v>916</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>917</v>
+        <v>921</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A299" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B299" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C299" s="2" t="s">
-        <v>94</v>
+        <v>891</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A300" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B300" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="C300" s="2" t="s">
-        <v>364</v>
+        <v>915</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A301" s="1" t="s">
-        <v>365</v>
+        <v>198</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>366</v>
+        <v>198</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A302" s="1" t="s">
-        <v>842</v>
+        <v>362</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>843</v>
+        <v>363</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>844</v>
+        <v>364</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A303" s="1" t="s">
-        <v>836</v>
+        <v>365</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>837</v>
+        <v>366</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.4">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A304" s="1" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A305" s="1" t="s">
-        <v>259</v>
+        <v>836</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>260</v>
+        <v>837</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>261</v>
+        <v>838</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A306" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="B306" s="1" t="s">
-        <v>846</v>
-      </c>
-      <c r="C306" s="1" t="s">
-        <v>847</v>
+        <v>839</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A307" s="1" t="s">
-        <v>410</v>
+        <v>259</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>411</v>
+        <v>260</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>412</v>
+        <v>261</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A308" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B308" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C308" s="2" t="s">
-        <v>273</v>
+        <v>845</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A309" s="1" t="s">
-        <v>309</v>
+        <v>410</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>310</v>
+        <v>411</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>311</v>
+        <v>412</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A310" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>935</v>
+        <v>273</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A311" s="1" t="s">
-        <v>229</v>
+        <v>309</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>230</v>
+        <v>310</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>231</v>
+        <v>311</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A312" s="1" t="s">
-        <v>950</v>
+        <v>274</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>954</v>
+        <v>275</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A313" s="1" t="s">
-        <v>882</v>
+        <v>229</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>883</v>
+        <v>230</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>884</v>
+        <v>231</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A314" s="1" t="s">
-        <v>244</v>
+        <v>950</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>245</v>
+        <v>954</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.4">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A315" s="1" t="s">
-        <v>238</v>
+        <v>882</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>239</v>
+        <v>883</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>240</v>
+        <v>884</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A316" s="1" t="s">
-        <v>146</v>
+        <v>244</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>147</v>
+        <v>245</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>148</v>
+        <v>246</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A317" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="B317" s="1" t="s">
-        <v>525</v>
+        <v>238</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>526</v>
+        <v>240</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A318" s="1" t="s">
-        <v>722</v>
+        <v>146</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>723</v>
+        <v>147</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>724</v>
+        <v>148</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A319" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="B319" s="2" t="s">
-        <v>720</v>
+        <v>524</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>721</v>
+        <v>526</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A320" s="1" t="s">
-        <v>506</v>
+        <v>722</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>507</v>
+        <v>723</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>508</v>
+        <v>724</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A321" s="1" t="s">
-        <v>482</v>
+        <v>719</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>483</v>
+        <v>720</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>484</v>
+        <v>721</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A322" s="1" t="s">
-        <v>476</v>
+        <v>506</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>477</v>
+        <v>507</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>478</v>
+        <v>508</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A323" s="1" t="s">
-        <v>626</v>
+        <v>482</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>627</v>
+        <v>483</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>628</v>
+        <v>484</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A324" s="1" t="s">
-        <v>518</v>
+        <v>476</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>519</v>
+        <v>477</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>520</v>
+        <v>478</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A325" s="1" t="s">
-        <v>189</v>
+        <v>626</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>189</v>
+        <v>627</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>66</v>
+        <v>628</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A326" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="B326" s="1" t="s">
-        <v>528</v>
+        <v>518</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>519</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A327" s="1" t="s">
-        <v>815</v>
+        <v>189</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>816</v>
+        <v>189</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>817</v>
+        <v>66</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A328" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B328" s="2" t="s">
-        <v>354</v>
+        <v>527</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>528</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>355</v>
+        <v>529</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A329" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A330" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A331" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B329" s="2" t="s">
+      <c r="B331" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C329" s="2" t="s">
+      <c r="C331" s="2" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B330" s="2"/>
-      <c r="C330" s="2"/>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B331" s="2"/>
-      <c r="C331" s="2"/>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B332" s="2"/>

</xml_diff>

<commit_message>
Add GET Jobs operation
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60518F0-7EB6-4126-9069-0EED45844602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914D9034-57E2-43E7-B5D3-4F57AC8B2460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6315" yWindow="720" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="1410" windowWidth="23085" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="973">
   <si>
     <t>Name</t>
   </si>
@@ -3221,6 +3221,30 @@
   </si>
   <si>
     <t>MachineNotFound</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JobConfigFilePath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jobs.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ジョブ.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FormJobOption</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ジョブ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3293,10 +3317,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C345" totalsRowShown="0">
-  <autoFilter ref="A1:C345" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C342">
-    <sortCondition ref="A1:A345"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C347" totalsRowShown="0">
+  <autoFilter ref="A1:C347" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C344">
+    <sortCondition ref="B1:B347"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
@@ -3570,10 +3594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C342"/>
+  <dimension ref="A1:C344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+    <sheetView tabSelected="1" topLeftCell="B83" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3596,519 +3620,519 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>220</v>
+        <v>760</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>221</v>
+        <v>761</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>222</v>
+        <v>762</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>262</v>
+        <v>500</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>263</v>
+        <v>501</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>264</v>
+        <v>502</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>223</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>224</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>225</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>220</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>425</v>
+        <v>226</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>426</v>
+        <v>227</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>427</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>419</v>
+        <v>262</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>420</v>
+        <v>263</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>421</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>637</v>
+        <v>341</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>638</v>
+        <v>342</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>639</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>634</v>
+        <v>497</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>635</v>
+        <v>498</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>636</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>464</v>
+        <v>940</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>465</v>
+        <v>942</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>466</v>
+        <v>945</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>422</v>
+        <v>941</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>423</v>
+        <v>943</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>424</v>
+        <v>944</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>416</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>417</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>418</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>185</v>
+        <v>419</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>185</v>
+        <v>420</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>288</v>
+        <v>637</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>289</v>
+        <v>638</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>290</v>
+        <v>639</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>408</v>
+        <v>422</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>423</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>409</v>
+        <v>424</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>256</v>
+        <v>416</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>257</v>
+        <v>417</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>258</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>936</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>937</v>
+        <v>407</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>938</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>932</v>
+        <v>185</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>933</v>
+        <v>185</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>939</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>297</v>
+        <v>143</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>298</v>
+        <v>144</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>299</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>849</v>
+        <v>936</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>938</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>893</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>894</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>895</v>
+        <v>932</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>928</v>
+        <v>256</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>530</v>
+        <v>297</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>531</v>
+        <v>298</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>532</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>522</v>
+        <v>306</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>523</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>517</v>
+        <v>847</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
+        <v>893</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>926</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>317</v>
+        <v>101</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>318</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>319</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>215</v>
+        <v>521</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>522</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>216</v>
+        <v>523</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>202</v>
+        <v>589</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>203</v>
+        <v>590</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.4">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>449</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>450</v>
+        <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>451</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>187</v>
+        <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>188</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>616</v>
+        <v>202</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>617</v>
+        <v>203</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>618</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>374</v>
+        <v>214</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>375</v>
+        <v>215</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>376</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>607</v>
+        <v>186</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>608</v>
+        <v>187</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>896</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A39" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>823</v>
+        <v>208</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>824</v>
+        <v>209</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>428</v>
+        <v>241</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>429</v>
+        <v>242</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>430</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>241</v>
+        <v>820</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>242</v>
+        <v>821</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>243</v>
+        <v>822</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>235</v>
+        <v>868</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>236</v>
+        <v>821</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>237</v>
+        <v>822</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>413</v>
+        <v>235</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>414</v>
+        <v>236</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>415</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="57.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>458</v>
+        <v>217</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>459</v>
+        <v>218</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>460</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>206</v>
+        <v>963</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>965</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>207</v>
+        <v>964</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>963</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>965</v>
+        <v>413</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>414</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>964</v>
+        <v>415</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.4">
@@ -4146,24 +4170,24 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>157</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>759</v>
+        <v>73</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
@@ -4190,112 +4214,112 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
-        <v>649</v>
+        <v>754</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>650</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>651</v>
+        <v>755</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>756</v>
+        <v>746</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
-        <v>745</v>
+        <v>192</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>746</v>
+        <v>192</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>747</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
-        <v>303</v>
+        <v>401</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>304</v>
+        <v>402</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>305</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
-        <v>300</v>
+        <v>727</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>301</v>
+        <v>728</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
-        <v>401</v>
+        <v>470</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>402</v>
+        <v>471</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>403</v>
+        <v>472</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
-        <v>727</v>
+        <v>98</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>728</v>
+        <v>99</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>729</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
-        <v>398</v>
+        <v>748</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>399</v>
+        <v>749</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>400</v>
+        <v>750</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.4">
@@ -4342,2479 +4366,2479 @@
         <v>684</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
-        <v>446</v>
+        <v>395</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>447</v>
+        <v>396</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>448</v>
+        <v>397</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
-        <v>395</v>
+        <v>568</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>396</v>
+        <v>569</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>397</v>
+        <v>570</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
-        <v>679</v>
+        <v>631</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>680</v>
+        <v>632</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>681</v>
+        <v>633</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>676</v>
+        <v>646</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>677</v>
+        <v>647</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>678</v>
+        <v>648</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
-        <v>164</v>
+        <v>706</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>165</v>
+        <v>707</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>166</v>
+        <v>708</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
-        <v>595</v>
+        <v>655</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>596</v>
+        <v>656</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>597</v>
+        <v>657</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
-        <v>583</v>
+        <v>658</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>584</v>
+        <v>659</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>585</v>
+        <v>660</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>167</v>
+        <v>688</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>168</v>
+        <v>689</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>169</v>
+        <v>690</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>724</v>
+        <v>697</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>725</v>
+        <v>698</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>726</v>
+        <v>699</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>383</v>
+        <v>715</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>384</v>
+        <v>716</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>385</v>
+        <v>717</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>586</v>
+        <v>679</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>587</v>
+        <v>680</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>588</v>
+        <v>681</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>580</v>
+        <v>676</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>581</v>
+        <v>677</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>53</v>
+        <v>338</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>53</v>
+        <v>339</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>5</v>
+        <v>808</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>6</v>
+        <v>809</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>7</v>
+        <v>810</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="75" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>134</v>
+        <v>392</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>135</v>
+        <v>393</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>136</v>
+        <v>394</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>940</v>
+        <v>380</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>942</v>
+        <v>381</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>945</v>
+        <v>382</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
-        <v>941</v>
+        <v>389</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>943</v>
+        <v>390</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>944</v>
+        <v>391</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>61</v>
+        <v>386</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>62</v>
+        <v>387</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>63</v>
+        <v>388</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
-        <v>101</v>
+        <v>583</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>102</v>
+        <v>584</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>103</v>
+        <v>585</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
-        <v>25</v>
+        <v>586</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>26</v>
+        <v>587</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
-        <v>131</v>
+        <v>598</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>132</v>
+        <v>599</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>133</v>
+        <v>600</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>16</v>
+        <v>580</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>17</v>
+        <v>581</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>18</v>
+        <v>582</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
-        <v>98</v>
+        <v>164</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>100</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
-        <v>52</v>
+        <v>199</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>53</v>
+        <v>200</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="93.75" x14ac:dyDescent="0.4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
-        <v>140</v>
+        <v>211</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>141</v>
+        <v>212</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>81</v>
+        <v>253</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>82</v>
+        <v>254</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>54</v>
+        <v>255</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
-        <v>89</v>
+        <v>247</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
-        <v>67</v>
+        <v>628</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>68</v>
+        <v>629</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>69</v>
+        <v>630</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
-        <v>13</v>
+        <v>539</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>14</v>
+        <v>540</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
-        <v>107</v>
+        <v>317</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>108</v>
+        <v>318</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
-        <v>104</v>
+        <v>323</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>46</v>
+        <v>320</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>47</v>
+        <v>321</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>48</v>
+        <v>322</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>11</v>
+        <v>344</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>12</v>
+        <v>345</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>12</v>
+        <v>346</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>8</v>
+        <v>960</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>9</v>
+        <v>961</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>10</v>
+        <v>962</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
-        <v>113</v>
+        <v>452</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>114</v>
+        <v>453</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>115</v>
+        <v>454</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
-        <v>79</v>
+        <v>455</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>80</v>
+        <v>456</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>51</v>
+        <v>457</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
-        <v>49</v>
+        <v>530</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>50</v>
+        <v>531</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>51</v>
+        <v>532</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
-        <v>86</v>
+        <v>437</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>87</v>
+        <v>438</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>88</v>
+        <v>439</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>40</v>
+        <v>440</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>41</v>
+        <v>441</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>119</v>
+        <v>431</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>120</v>
+        <v>432</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>121</v>
+        <v>433</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>76</v>
+        <v>643</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>77</v>
+        <v>644</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
-        <v>83</v>
+        <v>640</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>84</v>
+        <v>641</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
-        <v>70</v>
+        <v>473</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>71</v>
+        <v>474</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>72</v>
+        <v>475</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
-        <v>58</v>
+        <v>613</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>59</v>
+        <v>614</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>60</v>
+        <v>615</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
-        <v>95</v>
+        <v>428</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>96</v>
+        <v>429</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>97</v>
+        <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A120" s="1" t="s">
-        <v>31</v>
+        <v>434</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>32</v>
+        <v>435</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>33</v>
+        <v>436</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A121" s="1" t="s">
-        <v>28</v>
+        <v>398</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>29</v>
+        <v>399</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>30</v>
+        <v>400</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A122" s="1" t="s">
-        <v>125</v>
+        <v>515</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>126</v>
+        <v>516</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>127</v>
+        <v>517</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
-        <v>3</v>
+        <v>446</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>4</v>
+        <v>447</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="75" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
-        <v>92</v>
+        <v>449</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>93</v>
+        <v>450</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>94</v>
+        <v>451</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
-        <v>946</v>
+        <v>835</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>947</v>
+        <v>836</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A126" s="1" t="s">
-        <v>19</v>
+        <v>841</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>20</v>
+        <v>842</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>21</v>
+        <v>843</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A127" s="1" t="s">
-        <v>128</v>
+        <v>838</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>129</v>
+        <v>839</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>130</v>
+        <v>840</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A128" s="1" t="s">
-        <v>37</v>
+        <v>970</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>38</v>
+        <v>971</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>39</v>
+        <v>972</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
-        <v>116</v>
+        <v>967</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>117</v>
+        <v>968</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>118</v>
+        <v>969</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>65</v>
+        <v>357</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>66</v>
+        <v>358</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
-        <v>55</v>
+        <v>197</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>56</v>
+        <v>197</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>35</v>
+        <v>177</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>36</v>
+        <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
-        <v>211</v>
+        <v>957</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>212</v>
+        <v>958</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>213</v>
+        <v>959</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A135" s="1" t="s">
-        <v>253</v>
+        <v>954</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>254</v>
+        <v>955</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>255</v>
+        <v>956</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A136" s="1" t="s">
-        <v>199</v>
+        <v>67</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>200</v>
+        <v>68</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>201</v>
+        <v>69</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A137" s="1" t="s">
-        <v>247</v>
+        <v>563</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>248</v>
+        <v>564</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A138" s="1" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A139" s="1" t="s">
-        <v>628</v>
+        <v>574</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>629</v>
+        <v>575</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>630</v>
+        <v>576</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A140" s="1" t="s">
-        <v>539</v>
+        <v>966</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>540</v>
+        <v>566</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>541</v>
+        <v>567</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
-        <v>359</v>
+        <v>190</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>360</v>
+        <v>190</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>361</v>
+        <v>69</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A142" s="1" t="s">
-        <v>485</v>
+        <v>152</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>486</v>
+        <v>153</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>487</v>
+        <v>154</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A143" s="1" t="s">
-        <v>344</v>
+        <v>268</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>345</v>
+        <v>269</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>346</v>
+        <v>270</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A144" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>287</v>
+        <v>850</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="1" t="s">
-        <v>960</v>
+        <v>250</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>961</v>
+        <v>251</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>962</v>
+        <v>252</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A146" s="1" t="s">
-        <v>452</v>
+        <v>467</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>453</v>
+        <v>468</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>454</v>
+        <v>469</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A147" s="1" t="s">
-        <v>455</v>
+        <v>622</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>456</v>
+        <v>623</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A148" s="1" t="s">
-        <v>323</v>
+        <v>799</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>324</v>
+        <v>800</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>325</v>
+        <v>801</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A149" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>357</v>
+        <v>869</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>870</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>358</v>
+        <v>871</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A150" s="1" t="s">
-        <v>197</v>
+        <v>560</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>197</v>
+        <v>561</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>91</v>
+        <v>562</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A151" s="1" t="s">
-        <v>176</v>
+        <v>884</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>177</v>
+        <v>885</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>178</v>
+        <v>886</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A152" s="1" t="s">
-        <v>954</v>
+        <v>724</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>955</v>
+        <v>725</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="93.75" x14ac:dyDescent="0.4">
       <c r="A153" s="1" t="s">
-        <v>957</v>
+        <v>140</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>958</v>
+        <v>141</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>959</v>
+        <v>142</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A154" s="1" t="s">
-        <v>152</v>
+        <v>592</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>153</v>
+        <v>593</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>154</v>
+        <v>594</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A155" s="1" t="s">
-        <v>563</v>
+        <v>347</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>564</v>
+        <v>348</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>565</v>
+        <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="1" t="s">
-        <v>577</v>
+        <v>125</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>578</v>
+        <v>126</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>579</v>
+        <v>127</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A157" s="1" t="s">
-        <v>571</v>
+        <v>458</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>572</v>
+        <v>459</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>573</v>
+        <v>460</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="1" t="s">
-        <v>966</v>
+        <v>512</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>566</v>
+        <v>513</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>567</v>
+        <v>514</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A159" s="1" t="s">
-        <v>190</v>
+        <v>95</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>190</v>
+        <v>96</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A160" s="1" t="s">
-        <v>268</v>
+        <v>13</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>270</v>
+        <v>15</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A161" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>852</v>
+        <v>107</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A162" s="1" t="s">
-        <v>467</v>
+        <v>104</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>468</v>
+        <v>105</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>469</v>
+        <v>106</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A163" s="1" t="s">
-        <v>631</v>
+        <v>46</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>632</v>
+        <v>47</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>633</v>
+        <v>48</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A164" s="1" t="s">
-        <v>250</v>
+        <v>377</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>251</v>
+        <v>378</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A165" s="1" t="s">
-        <v>473</v>
+        <v>110</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>474</v>
+        <v>111</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>475</v>
+        <v>112</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A166" s="1" t="s">
-        <v>646</v>
+        <v>3</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>647</v>
+        <v>4</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>648</v>
+        <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A167" s="1" t="s">
-        <v>622</v>
+        <v>11</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>623</v>
+        <v>12</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>624</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A168" s="1" t="s">
-        <v>799</v>
+        <v>79</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>800</v>
+        <v>80</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>801</v>
+        <v>51</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A169" s="1" t="s">
-        <v>706</v>
+        <v>733</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>707</v>
+        <v>734</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>708</v>
+        <v>735</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A170" s="1" t="s">
-        <v>869</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>870</v>
+        <v>736</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>737</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>871</v>
+        <v>738</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A171" s="1" t="s">
-        <v>655</v>
+        <v>742</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>656</v>
+        <v>743</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>657</v>
+        <v>744</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A172" s="1" t="s">
-        <v>658</v>
+        <v>730</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>659</v>
+        <v>731</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>660</v>
+        <v>732</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A173" s="1" t="s">
-        <v>560</v>
+        <v>49</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>561</v>
+        <v>50</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A174" s="1" t="s">
-        <v>667</v>
+        <v>194</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>668</v>
+        <v>50</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>669</v>
+        <v>51</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A175" s="1" t="s">
-        <v>688</v>
+        <v>161</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>689</v>
+        <v>162</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>690</v>
+        <v>163</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A176" s="1" t="s">
-        <v>884</v>
+        <v>86</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>885</v>
+        <v>87</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>886</v>
+        <v>88</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A177" s="1" t="s">
-        <v>697</v>
+        <v>826</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>698</v>
+        <v>827</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>699</v>
+        <v>828</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A178" s="1" t="s">
-        <v>715</v>
+        <v>832</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>716</v>
+        <v>833</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>717</v>
+        <v>834</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A179" s="1" t="s">
-        <v>470</v>
+        <v>802</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>471</v>
+        <v>803</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>472</v>
+        <v>804</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A180" s="1" t="s">
-        <v>592</v>
+        <v>811</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>593</v>
+        <v>812</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A181" s="1" t="s">
-        <v>640</v>
+        <v>805</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>641</v>
+        <v>951</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>642</v>
+        <v>952</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A182" s="1" t="s">
-        <v>434</v>
+        <v>805</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>435</v>
+        <v>806</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A183" s="1" t="s">
-        <v>643</v>
+        <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>644</v>
+        <v>183</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>645</v>
+        <v>184</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
-        <v>437</v>
+        <v>196</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>438</v>
+        <v>196</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>439</v>
+        <v>88</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A185" s="1" t="s">
-        <v>440</v>
+        <v>823</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>441</v>
+        <v>824</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>442</v>
+        <v>825</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A186" s="1" t="s">
-        <v>350</v>
+        <v>173</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>351</v>
+        <v>174</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>352</v>
+        <v>175</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A187" s="1" t="s">
-        <v>766</v>
+        <v>312</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>767</v>
+        <v>313</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>768</v>
+        <v>314</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A188" s="1" t="s">
-        <v>598</v>
+        <v>40</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>599</v>
+        <v>41</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>600</v>
+        <v>42</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A189" s="1" t="s">
-        <v>574</v>
+        <v>461</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>575</v>
+        <v>462</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>576</v>
+        <v>463</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A190" s="1" t="s">
-        <v>389</v>
+        <v>119</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>390</v>
+        <v>120</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>391</v>
+        <v>121</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
-        <v>742</v>
+        <v>335</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>743</v>
+        <v>336</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>744</v>
+        <v>337</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
-        <v>793</v>
+        <v>137</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>794</v>
+        <v>138</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>795</v>
+        <v>139</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
-        <v>856</v>
+        <v>5</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>857</v>
+        <v>6</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>858</v>
+        <v>7</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
-        <v>554</v>
+        <v>76</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>555</v>
+        <v>77</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>556</v>
+        <v>78</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A195" s="1" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
-        <v>923</v>
+        <v>712</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>924</v>
+        <v>713</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>925</v>
+        <v>714</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
-        <v>503</v>
+        <v>775</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>504</v>
+        <v>776</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>505</v>
+        <v>777</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
-        <v>347</v>
+        <v>793</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>348</v>
+        <v>794</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>349</v>
+        <v>795</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
-        <v>817</v>
+        <v>784</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>818</v>
+        <v>785</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>819</v>
+        <v>786</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A200" s="1" t="s">
-        <v>512</v>
+        <v>787</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>513</v>
+        <v>788</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>514</v>
+        <v>789</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
-        <v>613</v>
+        <v>781</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>614</v>
+        <v>782</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>615</v>
+        <v>783</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
-        <v>332</v>
+        <v>193</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>333</v>
+        <v>193</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>334</v>
+        <v>78</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
-        <v>329</v>
+        <v>158</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>330</v>
+        <v>159</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>331</v>
+        <v>160</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
-        <v>279</v>
+        <v>315</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>280</v>
+        <v>935</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>281</v>
+        <v>316</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A205" s="1" t="s">
-        <v>377</v>
+        <v>83</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>378</v>
+        <v>84</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>379</v>
+        <v>85</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>277</v>
+        <v>872</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>873</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>278</v>
+        <v>874</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
-        <v>619</v>
+        <v>664</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>620</v>
+        <v>665</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>621</v>
+        <v>666</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A208" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>284</v>
+        <v>859</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>861</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
-        <v>161</v>
+        <v>856</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>162</v>
+        <v>857</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>163</v>
+        <v>858</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
-        <v>194</v>
+        <v>875</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>50</v>
+        <v>876</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>51</v>
+        <v>877</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
-        <v>497</v>
+        <v>878</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>498</v>
+        <v>879</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>499</v>
+        <v>880</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A212" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>394</v>
+        <v>853</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>381</v>
+        <v>195</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>382</v>
+        <v>85</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
-        <v>386</v>
+        <v>170</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>387</v>
+        <v>171</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A215" s="1" t="s">
-        <v>739</v>
+        <v>70</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>740</v>
+        <v>71</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
-        <v>733</v>
+        <v>533</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>734</v>
+        <v>534</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>735</v>
+        <v>535</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
-        <v>736</v>
+        <v>548</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>737</v>
+        <v>549</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>738</v>
+        <v>550</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
-        <v>730</v>
+        <v>694</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>731</v>
+        <v>695</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>732</v>
+        <v>696</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
-        <v>832</v>
+        <v>542</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>833</v>
+        <v>543</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>834</v>
+        <v>544</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
-        <v>173</v>
+        <v>554</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>174</v>
+        <v>555</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>175</v>
+        <v>556</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A221" s="1" t="s">
-        <v>826</v>
+        <v>536</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>827</v>
+        <v>537</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>828</v>
+        <v>538</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A222" s="1" t="s">
-        <v>182</v>
+        <v>545</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>183</v>
+        <v>546</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>184</v>
+        <v>547</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A223" s="1" t="s">
-        <v>820</v>
+        <v>191</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>821</v>
+        <v>191</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>822</v>
+        <v>72</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A224" s="1" t="s">
-        <v>808</v>
+        <v>149</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>809</v>
+        <v>150</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>810</v>
+        <v>151</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A225" s="1" t="s">
-        <v>802</v>
+        <v>601</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>803</v>
+        <v>602</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>804</v>
+        <v>603</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A226" s="1" t="s">
-        <v>811</v>
+        <v>604</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>812</v>
+        <v>605</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>813</v>
+        <v>606</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A227" s="1" t="s">
-        <v>196</v>
+        <v>772</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>196</v>
+        <v>773</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>88</v>
+        <v>774</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A228" s="1" t="s">
-        <v>805</v>
+        <v>769</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>951</v>
+        <v>770</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>952</v>
+        <v>771</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A229" s="1" t="s">
-        <v>805</v>
+        <v>610</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>806</v>
+        <v>611</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>807</v>
+        <v>612</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A230" s="1" t="s">
-        <v>312</v>
+        <v>232</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>313</v>
+        <v>233</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>314</v>
+        <v>234</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A231" s="1" t="s">
-        <v>461</v>
+        <v>58</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>462</v>
+        <v>59</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>463</v>
+        <v>60</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A232" s="1" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>336</v>
+        <v>369</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>337</v>
+        <v>370</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A233" s="1" t="s">
-        <v>431</v>
+        <v>829</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>432</v>
+        <v>830</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>433</v>
+        <v>831</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A234" s="1" t="s">
-        <v>158</v>
+        <v>634</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>159</v>
+        <v>635</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>160</v>
+        <v>636</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A235" s="1" t="s">
-        <v>341</v>
+        <v>616</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>342</v>
+        <v>617</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A236" s="1" t="s">
-        <v>533</v>
+        <v>649</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>534</v>
+        <v>650</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A237" s="1" t="s">
-        <v>338</v>
+        <v>709</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>339</v>
+        <v>710</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>340</v>
+        <v>711</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A238" s="1" t="s">
-        <v>193</v>
+        <v>661</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>193</v>
+        <v>662</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>78</v>
+        <v>663</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A239" s="1" t="s">
-        <v>790</v>
+        <v>691</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>791</v>
+        <v>692</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>792</v>
+        <v>693</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A240" s="1" t="s">
-        <v>778</v>
+        <v>700</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>779</v>
+        <v>701</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>780</v>
+        <v>702</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A241" s="1" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>714</v>
+        <v>720</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A242" s="1" t="s">
-        <v>709</v>
+        <v>619</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>710</v>
+        <v>620</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>711</v>
+        <v>621</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A243" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>797</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>798</v>
+        <v>902</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>904</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A244" s="1" t="s">
-        <v>775</v>
+        <v>479</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>776</v>
+        <v>480</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>777</v>
+        <v>481</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A245" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="B245" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="C245" s="2" t="s">
-        <v>783</v>
+        <v>905</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>907</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A246" s="1" t="s">
-        <v>784</v>
+        <v>276</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>785</v>
+        <v>277</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>786</v>
+        <v>278</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A247" s="1" t="s">
-        <v>787</v>
+        <v>488</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>788</v>
+        <v>489</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>789</v>
+        <v>490</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A248" s="1" t="s">
-        <v>315</v>
+        <v>31</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>935</v>
+        <v>32</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>316</v>
+        <v>33</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A249" s="1" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>172</v>
+        <v>30</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A250" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>873</v>
+        <v>464</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>465</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>874</v>
+        <v>466</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A251" s="1" t="s">
-        <v>868</v>
+        <v>763</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>821</v>
+        <v>764</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>822</v>
+        <v>765</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A252" s="1" t="s">
-        <v>862</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>863</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>864</v>
+        <v>265</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A253" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="B253" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>666</v>
+        <v>862</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A254" s="1" t="s">
-        <v>661</v>
+        <v>383</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>662</v>
+        <v>384</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>663</v>
+        <v>385</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A255" s="1" t="s">
-        <v>865</v>
+        <v>350</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>866</v>
+        <v>351</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>867</v>
+        <v>352</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A256" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>861</v>
+        <v>796</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A257" s="1" t="s">
-        <v>853</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>854</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>855</v>
+        <v>865</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>867</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A258" s="1" t="s">
-        <v>875</v>
+        <v>557</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>876</v>
+        <v>558</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.4">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A259" s="1" t="s">
-        <v>878</v>
+        <v>326</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>879</v>
+        <v>327</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>880</v>
+        <v>328</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A260" s="1" t="s">
-        <v>195</v>
+        <v>425</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>195</v>
+        <v>426</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>85</v>
+        <v>427</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A261" s="1" t="s">
-        <v>760</v>
+        <v>410</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>761</v>
+        <v>411</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>762</v>
+        <v>412</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A262" s="1" t="s">
-        <v>149</v>
+        <v>374</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>150</v>
+        <v>375</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>151</v>
+        <v>376</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A263" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="B263" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C263" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>757</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A264" s="1" t="s">
-        <v>748</v>
+        <v>595</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>749</v>
+        <v>596</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>750</v>
+        <v>597</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A265" s="1" t="s">
-        <v>551</v>
+        <v>359</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>552</v>
+        <v>360</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>553</v>
+        <v>361</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A266" s="1" t="s">
-        <v>548</v>
+        <v>485</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>549</v>
+        <v>486</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>550</v>
+        <v>487</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A267" s="1" t="s">
-        <v>694</v>
+        <v>577</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>695</v>
+        <v>578</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>696</v>
+        <v>579</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A268" s="1" t="s">
-        <v>691</v>
+        <v>817</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>692</v>
+        <v>818</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>693</v>
+        <v>819</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A269" s="1" t="s">
-        <v>557</v>
+        <v>282</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>558</v>
+        <v>283</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.4">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A270" s="1" t="s">
-        <v>542</v>
+        <v>285</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>543</v>
+        <v>286</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>544</v>
+        <v>287</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A271" s="1" t="s">
-        <v>536</v>
+        <v>288</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>537</v>
+        <v>289</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.4">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A272" s="1" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>191</v>
+        <v>292</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>72</v>
+        <v>293</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A273" s="1" t="s">
-        <v>545</v>
+        <v>279</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>546</v>
+        <v>280</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.4">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A274" s="1" t="s">
-        <v>500</v>
+        <v>739</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>501</v>
+        <v>740</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>502</v>
+        <v>741</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A275" s="1" t="s">
-        <v>601</v>
+        <v>790</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>602</v>
+        <v>791</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>603</v>
+        <v>792</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A276" s="1" t="s">
-        <v>604</v>
+        <v>551</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>605</v>
+        <v>552</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>606</v>
+        <v>553</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A277" s="1" t="s">
-        <v>769</v>
+        <v>371</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>770</v>
+        <v>372</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>771</v>
+        <v>373</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A278" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="B278" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>612</v>
+        <v>911</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A279" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B279" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>234</v>
+        <v>917</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A280" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A281" s="1" t="s">
-        <v>371</v>
+        <v>814</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>372</v>
+        <v>815</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>373</v>
+        <v>816</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A282" s="1" t="s">
-        <v>829</v>
+        <v>920</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>830</v>
+        <v>921</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A283" s="1" t="s">
-        <v>320</v>
+        <v>506</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>321</v>
+        <v>507</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.4">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A284" s="1" t="s">
-        <v>896</v>
-      </c>
-      <c r="B284" s="1" t="s">
-        <v>897</v>
-      </c>
-      <c r="C284" s="1" t="s">
-        <v>898</v>
+        <v>303</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A285" s="1" t="s">
-        <v>899</v>
-      </c>
-      <c r="B285" s="1" t="s">
-        <v>900</v>
-      </c>
-      <c r="C285" s="1" t="s">
-        <v>901</v>
+        <v>300</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A286" s="1" t="s">
-        <v>911</v>
-      </c>
-      <c r="B286" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C286" s="1" t="s">
-        <v>913</v>
+        <v>607</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A287" s="1" t="s">
-        <v>902</v>
+        <v>908</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>903</v>
+        <v>909</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>904</v>
+        <v>910</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A288" s="1" t="s">
-        <v>479</v>
+        <v>92</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>480</v>
+        <v>93</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>481</v>
+        <v>94</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A289" s="1" t="s">
-        <v>265</v>
+        <v>887</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>266</v>
+        <v>888</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>267</v>
+        <v>889</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A290" s="1" t="s">
-        <v>905</v>
-      </c>
-      <c r="B290" s="1" t="s">
-        <v>906</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>907</v>
+        <v>703</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A291" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="B291" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="C291" s="2" t="s">
-        <v>490</v>
+        <v>890</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>892</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A292" s="1" t="s">
-        <v>908</v>
-      </c>
-      <c r="B292" s="1" t="s">
-        <v>909</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>910</v>
+        <v>923</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>925</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A293" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B293" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>914</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A294" s="1" t="s">
-        <v>294</v>
+        <v>198</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>295</v>
+        <v>198</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>296</v>
+        <v>94</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.4">
@@ -6830,398 +6854,398 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A296" s="1" t="s">
-        <v>917</v>
-      </c>
-      <c r="B296" s="1" t="s">
-        <v>918</v>
-      </c>
-      <c r="C296" s="1" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.4">
+        <v>362</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A297" s="1" t="s">
-        <v>887</v>
+        <v>294</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>888</v>
+        <v>295</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>889</v>
+        <v>296</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A298" s="1" t="s">
-        <v>703</v>
+        <v>259</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>704</v>
+        <v>260</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.4">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" ht="75" x14ac:dyDescent="0.4">
       <c r="A299" s="1" t="s">
-        <v>700</v>
+        <v>134</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>701</v>
+        <v>135</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A300" s="1" t="s">
-        <v>920</v>
+        <v>128</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>921</v>
+        <v>129</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>922</v>
+        <v>130</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A301" s="1" t="s">
-        <v>890</v>
+        <v>844</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>891</v>
+        <v>845</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>892</v>
+        <v>846</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A302" s="1" t="s">
-        <v>914</v>
-      </c>
-      <c r="B302" s="1" t="s">
-        <v>915</v>
-      </c>
-      <c r="C302" s="1" t="s">
-        <v>916</v>
+        <v>271</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A303" s="1" t="s">
-        <v>198</v>
+        <v>309</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>198</v>
+        <v>310</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>94</v>
+        <v>311</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A304" s="1" t="s">
-        <v>362</v>
+        <v>274</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>363</v>
+        <v>275</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>364</v>
+        <v>934</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A305" s="1" t="s">
-        <v>365</v>
+        <v>229</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>366</v>
+        <v>230</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A306" s="1" t="s">
-        <v>841</v>
+        <v>949</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>842</v>
+        <v>953</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>843</v>
+        <v>950</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A307" s="1" t="s">
-        <v>835</v>
+        <v>244</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>836</v>
+        <v>245</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A308" s="1" t="s">
-        <v>838</v>
+        <v>881</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>839</v>
+        <v>882</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>840</v>
+        <v>883</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A309" s="1" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A310" s="1" t="s">
-        <v>844</v>
+        <v>122</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>845</v>
+        <v>123</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>846</v>
+        <v>124</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A311" s="1" t="s">
-        <v>410</v>
+        <v>55</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>411</v>
+        <v>56</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>412</v>
+        <v>57</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A312" s="1" t="s">
-        <v>271</v>
+        <v>946</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>272</v>
+        <v>947</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>273</v>
+        <v>948</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A313" s="1" t="s">
-        <v>309</v>
+        <v>64</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>310</v>
+        <v>65</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>311</v>
+        <v>66</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A314" s="1" t="s">
-        <v>274</v>
+        <v>625</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>275</v>
+        <v>626</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.4">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A315" s="1" t="s">
-        <v>229</v>
+        <v>667</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>230</v>
+        <v>668</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>231</v>
+        <v>669</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A316" s="1" t="s">
-        <v>949</v>
+        <v>332</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>953</v>
+        <v>333</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A317" s="1" t="s">
-        <v>881</v>
+        <v>329</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>882</v>
+        <v>330</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>883</v>
+        <v>331</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A318" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>245</v>
+        <v>524</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>246</v>
+        <v>526</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A319" s="1" t="s">
-        <v>238</v>
+        <v>19</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>239</v>
+        <v>20</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>240</v>
+        <v>21</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A320" s="1" t="s">
-        <v>146</v>
+        <v>721</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>147</v>
+        <v>722</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>148</v>
+        <v>723</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A321" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="B321" s="1" t="s">
-        <v>525</v>
+        <v>476</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>477</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>526</v>
+        <v>478</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A322" s="1" t="s">
-        <v>721</v>
+        <v>518</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>722</v>
+        <v>519</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>723</v>
+        <v>520</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A323" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="B323" s="2" t="s">
-        <v>719</v>
+        <v>527</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>528</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>720</v>
+        <v>529</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A324" s="1" t="s">
-        <v>506</v>
+        <v>37</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>507</v>
+        <v>38</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>508</v>
+        <v>39</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A325" s="1" t="s">
-        <v>482</v>
+        <v>503</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>483</v>
+        <v>504</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>484</v>
+        <v>505</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A326" s="1" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A327" s="1" t="s">
-        <v>625</v>
+        <v>116</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>626</v>
+        <v>117</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>627</v>
+        <v>118</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A328" s="1" t="s">
-        <v>518</v>
+        <v>189</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>519</v>
+        <v>189</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>520</v>
+        <v>66</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A329" s="1" t="s">
-        <v>189</v>
+        <v>509</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>189</v>
+        <v>510</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>66</v>
+        <v>511</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A330" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="B330" s="1" t="s">
-        <v>528</v>
+        <v>146</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>529</v>
+        <v>148</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A331" s="1" t="s">
-        <v>814</v>
+        <v>8</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>815</v>
+        <v>9</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>816</v>
+        <v>10</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.4">
@@ -7237,34 +7261,56 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A333" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A334" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B333" s="2" t="s">
+      <c r="B334" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C333" s="2" t="s">
+      <c r="C334" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B334" s="2"/>
-      <c r="C334" s="2"/>
-    </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B335" s="2"/>
-      <c r="C335" s="2"/>
+      <c r="A335" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
     </row>
-    <row r="341" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B341" s="2"/>
-      <c r="C341" s="2"/>
-    </row>
-    <row r="342" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B342" s="2"/>
-      <c r="C342" s="2"/>
+    <row r="337" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B337" s="2"/>
+      <c r="C337" s="2"/>
+    </row>
+    <row r="338" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B338" s="2"/>
+      <c r="C338" s="2"/>
+    </row>
+    <row r="343" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B343" s="2"/>
+      <c r="C343" s="2"/>
+    </row>
+    <row r="344" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B344" s="2"/>
+      <c r="C344" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Handled duplicate library/package versions in Orchestrator
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/andra_dregan_uipath_com/Documents/Documents/UiPath/OrchestratorManager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914D9034-57E2-43E7-B5D3-4F57AC8B2460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{914D9034-57E2-43E7-B5D3-4F57AC8B2460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E7E793E-ED53-44BF-B658-9C799E644351}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="1410" windowWidth="23085" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="982">
   <si>
     <t>Name</t>
   </si>
@@ -3247,22 +3247,57 @@
     <t>ジョブ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>DuplicatedLibrary</t>
+  </si>
+  <si>
+    <t>DuplicatedPackage</t>
+  </si>
+  <si>
+    <t>Duplicated library version found in Orchestrator for:
+{0}
+- and will be skipped from processing. Please check these entities manually.</t>
+  </si>
+  <si>
+    <t>Orchestratorで見つかった複製ライブラリバージョン：
+{0}
+-そして処理からスキップされます。 これらのエンティティを手動で確認してください。</t>
+  </si>
+  <si>
+    <t>Orchestratorで見つかった重複パッケージバージョン：
+{0}
+-そして、それは処理からスキップされます。 これらのエンティティを手動で確認してください。</t>
+  </si>
+  <si>
+    <t>Duplicated package version found in Orchestrator for:
+{0}
+- and will be skipped from processing. Please check these entities manually.</t>
+  </si>
+  <si>
+    <t>NoUniquePackageOrLibrary</t>
+  </si>
+  <si>
+    <t>No unique package/library versions found</t>
+  </si>
+  <si>
+    <t>一意のパッケージ/ライブラリバージョンが見つかりません</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3317,10 +3352,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C347" totalsRowShown="0">
-  <autoFilter ref="A1:C347" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C344">
-    <sortCondition ref="B1:B347"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table13" displayName="Table13" ref="A1:C345" totalsRowShown="0">
+  <autoFilter ref="A1:C345" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C342">
+    <sortCondition ref="B1:B345"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
@@ -3594,20 +3629,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
-  <dimension ref="A1:C344"/>
+  <dimension ref="A1:C342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B83" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="50.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="84.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="84.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3618,7 +3653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>760</v>
       </c>
@@ -3629,7 +3664,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="43.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>500</v>
       </c>
@@ -3640,7 +3675,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -3651,7 +3686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>223</v>
       </c>
@@ -3662,7 +3697,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>220</v>
       </c>
@@ -3673,7 +3708,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>226</v>
       </c>
@@ -3684,7 +3719,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>262</v>
       </c>
@@ -3695,7 +3730,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>341</v>
       </c>
@@ -3706,7 +3741,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>497</v>
       </c>
@@ -3717,7 +3752,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>940</v>
       </c>
@@ -3728,7 +3763,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>941</v>
       </c>
@@ -3739,7 +3774,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
@@ -3750,7 +3785,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>419</v>
       </c>
@@ -3761,7 +3796,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>637</v>
       </c>
@@ -3772,7 +3807,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>422</v>
       </c>
@@ -3783,7 +3818,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>416</v>
       </c>
@@ -3794,7 +3829,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>407</v>
       </c>
@@ -3805,7 +3840,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>185</v>
       </c>
@@ -3816,7 +3851,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="30" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>143</v>
       </c>
@@ -3827,7 +3862,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>936</v>
       </c>
@@ -3838,7 +3873,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>932</v>
       </c>
@@ -3849,7 +3884,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>256</v>
       </c>
@@ -3860,7 +3895,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>297</v>
       </c>
@@ -3871,7 +3906,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>306</v>
       </c>
@@ -3882,7 +3917,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>847</v>
       </c>
@@ -3893,7 +3928,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>893</v>
       </c>
@@ -3904,7 +3939,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>926</v>
       </c>
@@ -3915,7 +3950,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>101</v>
       </c>
@@ -3926,7 +3961,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>521</v>
       </c>
@@ -3937,7 +3972,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>589</v>
       </c>
@@ -3948,7 +3983,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3959,7 +3994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -3970,7 +4005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>202</v>
       </c>
@@ -3981,7 +4016,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>214</v>
       </c>
@@ -3992,7 +4027,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>186</v>
       </c>
@@ -4003,7 +4038,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>896</v>
       </c>
@@ -4014,7 +4049,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>899</v>
       </c>
@@ -4025,7 +4060,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="28.8">
       <c r="A39" s="1" t="s">
         <v>443</v>
       </c>
@@ -4036,7 +4071,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>208</v>
       </c>
@@ -4047,7 +4082,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>241</v>
       </c>
@@ -4058,7 +4093,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
         <v>820</v>
       </c>
@@ -4069,7 +4104,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="43.5" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>868</v>
       </c>
@@ -4080,7 +4115,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="43.5" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>235</v>
       </c>
@@ -4091,7 +4126,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="57.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="57.9" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>205</v>
       </c>
@@ -4102,7 +4137,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" ht="54" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>217</v>
       </c>
@@ -4113,7 +4148,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" ht="135" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>963</v>
       </c>
@@ -4124,7 +4159,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" ht="28.8">
       <c r="A48" s="1" t="s">
         <v>413</v>
       </c>
@@ -4135,7 +4170,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" ht="90" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>494</v>
       </c>
@@ -4146,7 +4181,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
         <v>491</v>
       </c>
@@ -4157,7 +4192,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>929</v>
       </c>
@@ -4168,7 +4203,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
@@ -4179,7 +4214,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>73</v>
       </c>
@@ -4190,7 +4225,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
         <v>751</v>
       </c>
@@ -4201,7 +4236,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
         <v>652</v>
       </c>
@@ -4212,7 +4247,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
         <v>754</v>
       </c>
@@ -4223,7 +4258,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
         <v>766</v>
       </c>
@@ -4234,7 +4269,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
         <v>745</v>
       </c>
@@ -4245,7 +4280,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>192</v>
       </c>
@@ -4256,7 +4291,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
         <v>155</v>
       </c>
@@ -4267,7 +4302,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
         <v>401</v>
       </c>
@@ -4278,7 +4313,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
         <v>727</v>
       </c>
@@ -4289,7 +4324,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3" ht="28.8">
       <c r="A63" s="1" t="s">
         <v>470</v>
       </c>
@@ -4300,7 +4335,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" ht="18">
       <c r="A64" s="1" t="s">
         <v>98</v>
       </c>
@@ -4311,7 +4346,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" ht="28.8">
       <c r="A65" s="1" t="s">
         <v>748</v>
       </c>
@@ -4322,7 +4357,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
         <v>673</v>
       </c>
@@ -4333,7 +4368,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
         <v>670</v>
       </c>
@@ -4344,7 +4379,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
         <v>685</v>
       </c>
@@ -4355,7 +4390,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
         <v>682</v>
       </c>
@@ -4366,7 +4401,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" ht="28.8">
       <c r="A70" s="1" t="s">
         <v>395</v>
       </c>
@@ -4377,7 +4412,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" ht="28.8">
       <c r="A71" s="1" t="s">
         <v>568</v>
       </c>
@@ -4388,7 +4423,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
         <v>631</v>
       </c>
@@ -4399,7 +4434,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
         <v>646</v>
       </c>
@@ -4410,7 +4445,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
         <v>706</v>
       </c>
@@ -4421,7 +4456,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
         <v>655</v>
       </c>
@@ -4432,7 +4467,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
         <v>658</v>
       </c>
@@ -4443,7 +4478,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
         <v>688</v>
       </c>
@@ -4454,7 +4489,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
         <v>697</v>
       </c>
@@ -4465,7 +4500,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
         <v>715</v>
       </c>
@@ -4476,7 +4511,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
         <v>679</v>
       </c>
@@ -4487,7 +4522,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
         <v>676</v>
       </c>
@@ -4498,7 +4533,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" ht="28.8">
       <c r="A82" s="1" t="s">
         <v>338</v>
       </c>
@@ -4509,7 +4544,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
         <v>808</v>
       </c>
@@ -4520,7 +4555,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
@@ -4531,7 +4566,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
         <v>392</v>
       </c>
@@ -4542,7 +4577,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
         <v>380</v>
       </c>
@@ -4553,7 +4588,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
         <v>389</v>
       </c>
@@ -4564,7 +4599,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
         <v>386</v>
       </c>
@@ -4575,7 +4610,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
         <v>583</v>
       </c>
@@ -4586,7 +4621,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3">
       <c r="A90" s="1" t="s">
         <v>586</v>
       </c>
@@ -4597,7 +4632,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
         <v>598</v>
       </c>
@@ -4608,7 +4643,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
         <v>580</v>
       </c>
@@ -4619,7 +4654,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
         <v>167</v>
       </c>
@@ -4630,7 +4665,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3">
       <c r="A94" s="1" t="s">
         <v>53</v>
       </c>
@@ -4641,7 +4676,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
         <v>52</v>
       </c>
@@ -4652,7 +4687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
         <v>164</v>
       </c>
@@ -4663,7 +4698,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
         <v>199</v>
       </c>
@@ -4674,7 +4709,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
         <v>211</v>
       </c>
@@ -4685,7 +4720,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
         <v>253</v>
       </c>
@@ -4696,7 +4731,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:3">
       <c r="A100" s="1" t="s">
         <v>247</v>
       </c>
@@ -4707,7 +4742,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>628</v>
       </c>
@@ -4718,7 +4753,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:3">
       <c r="A102" s="1" t="s">
         <v>539</v>
       </c>
@@ -4729,7 +4764,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:3" ht="28.8">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -4740,7 +4775,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:3" ht="28.8">
       <c r="A104" s="1" t="s">
         <v>323</v>
       </c>
@@ -4751,7 +4786,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:3" ht="28.8">
       <c r="A105" s="1" t="s">
         <v>320</v>
       </c>
@@ -4762,7 +4797,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:3">
       <c r="A106" s="1" t="s">
         <v>344</v>
       </c>
@@ -4773,7 +4808,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:3" ht="45" customHeight="1">
       <c r="A107" s="1" t="s">
         <v>131</v>
       </c>
@@ -4784,7 +4819,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:3" ht="45" customHeight="1">
       <c r="A108" s="1" t="s">
         <v>960</v>
       </c>
@@ -4795,7 +4830,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:3" ht="45" customHeight="1">
       <c r="A109" s="1" t="s">
         <v>452</v>
       </c>
@@ -4806,7 +4841,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:3" ht="29.1" customHeight="1">
       <c r="A110" s="1" t="s">
         <v>455</v>
       </c>
@@ -4817,7 +4852,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:3" ht="36" customHeight="1">
       <c r="A111" s="1" t="s">
         <v>530</v>
       </c>
@@ -4828,7 +4863,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:3" ht="36" customHeight="1">
       <c r="A112" s="1" t="s">
         <v>437</v>
       </c>
@@ -4839,7 +4874,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:3" ht="29.1" customHeight="1">
       <c r="A113" s="1" t="s">
         <v>440</v>
       </c>
@@ -4850,7 +4885,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:3" ht="28.8">
       <c r="A114" s="1" t="s">
         <v>431</v>
       </c>
@@ -4861,7 +4896,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:3" ht="36" customHeight="1">
       <c r="A115" s="1" t="s">
         <v>643</v>
       </c>
@@ -4872,7 +4907,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:3" ht="28.8">
       <c r="A116" s="1" t="s">
         <v>640</v>
       </c>
@@ -4883,7 +4918,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:3" ht="28.8">
       <c r="A117" s="1" t="s">
         <v>473</v>
       </c>
@@ -4894,7 +4929,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:3" ht="30" customHeight="1">
       <c r="A118" s="1" t="s">
         <v>613</v>
       </c>
@@ -4905,7 +4940,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:3" ht="29.1" customHeight="1">
       <c r="A119" s="1" t="s">
         <v>428</v>
       </c>
@@ -4916,7 +4951,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:3" ht="29.1" customHeight="1">
       <c r="A120" s="1" t="s">
         <v>434</v>
       </c>
@@ -4927,7 +4962,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:3" ht="43.5" customHeight="1">
       <c r="A121" s="1" t="s">
         <v>398</v>
       </c>
@@ -4938,7 +4973,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:3" ht="30" customHeight="1">
       <c r="A122" s="1" t="s">
         <v>515</v>
       </c>
@@ -4949,7 +4984,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:3" ht="54" customHeight="1">
       <c r="A123" s="1" t="s">
         <v>446</v>
       </c>
@@ -4960,7 +4995,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="75" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:3" ht="57.6">
       <c r="A124" s="1" t="s">
         <v>449</v>
       </c>
@@ -4971,7 +5006,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:3" ht="29.1" customHeight="1">
       <c r="A125" s="1" t="s">
         <v>835</v>
       </c>
@@ -4982,7 +5017,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:3" ht="28.8">
       <c r="A126" s="1" t="s">
         <v>841</v>
       </c>
@@ -4993,7 +5028,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:3" ht="36" customHeight="1">
       <c r="A127" s="1" t="s">
         <v>838</v>
       </c>
@@ -5004,7 +5039,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:3">
       <c r="A128" s="1" t="s">
         <v>970</v>
       </c>
@@ -5015,7 +5050,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
         <v>967</v>
       </c>
@@ -5026,7 +5061,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
         <v>356</v>
       </c>
@@ -5037,7 +5072,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
         <v>197</v>
       </c>
@@ -5048,7 +5083,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:3">
       <c r="A132" s="1" t="s">
         <v>176</v>
       </c>
@@ -5059,7 +5094,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:3">
       <c r="A133" s="1" t="s">
         <v>89</v>
       </c>
@@ -5070,7 +5105,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:3">
       <c r="A134" s="1" t="s">
         <v>957</v>
       </c>
@@ -5081,7 +5116,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:3">
       <c r="A135" s="1" t="s">
         <v>954</v>
       </c>
@@ -5092,7 +5127,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:3">
       <c r="A136" s="1" t="s">
         <v>67</v>
       </c>
@@ -5103,7 +5138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:3">
       <c r="A137" s="1" t="s">
         <v>563</v>
       </c>
@@ -5114,7 +5149,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:3">
       <c r="A138" s="1" t="s">
         <v>571</v>
       </c>
@@ -5125,7 +5160,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:3">
       <c r="A139" s="1" t="s">
         <v>574</v>
       </c>
@@ -5136,7 +5171,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:3">
       <c r="A140" s="1" t="s">
         <v>966</v>
       </c>
@@ -5147,7 +5182,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:3">
       <c r="A141" s="1" t="s">
         <v>190</v>
       </c>
@@ -5158,7 +5193,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:3">
       <c r="A142" s="1" t="s">
         <v>152</v>
       </c>
@@ -5169,7 +5204,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:3" ht="29.1" customHeight="1">
       <c r="A143" s="1" t="s">
         <v>268</v>
       </c>
@@ -5180,7 +5215,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:3" ht="29.1" customHeight="1">
       <c r="A144" s="1" t="s">
         <v>850</v>
       </c>
@@ -5191,7 +5226,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:3" ht="29.1" customHeight="1">
       <c r="A145" s="1" t="s">
         <v>250</v>
       </c>
@@ -5202,7 +5237,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:3" ht="36" customHeight="1">
       <c r="A146" s="1" t="s">
         <v>467</v>
       </c>
@@ -5213,7 +5248,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:3" ht="36" customHeight="1">
       <c r="A147" s="1" t="s">
         <v>622</v>
       </c>
@@ -5224,7 +5259,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:3">
       <c r="A148" s="1" t="s">
         <v>799</v>
       </c>
@@ -5235,7 +5270,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
         <v>869</v>
       </c>
@@ -5246,7 +5281,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:3" ht="29.1" customHeight="1">
       <c r="A150" s="1" t="s">
         <v>560</v>
       </c>
@@ -5257,7 +5292,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:3">
       <c r="A151" s="1" t="s">
         <v>884</v>
       </c>
@@ -5268,7 +5303,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:3">
       <c r="A152" s="1" t="s">
         <v>724</v>
       </c>
@@ -5279,7 +5314,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="93.75" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:3" ht="72">
       <c r="A153" s="1" t="s">
         <v>140</v>
       </c>
@@ -5290,7 +5325,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:3">
       <c r="A154" s="1" t="s">
         <v>592</v>
       </c>
@@ -5301,7 +5336,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:3" ht="30" customHeight="1">
       <c r="A155" s="1" t="s">
         <v>347</v>
       </c>
@@ -5312,7 +5347,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:3" ht="30" customHeight="1">
       <c r="A156" s="1" t="s">
         <v>125</v>
       </c>
@@ -5323,7 +5358,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:3" ht="30" customHeight="1">
       <c r="A157" s="1" t="s">
         <v>458</v>
       </c>
@@ -5334,7 +5369,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:3" ht="30" customHeight="1">
       <c r="A158" s="1" t="s">
         <v>512</v>
       </c>
@@ -5345,7 +5380,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:3" ht="30" customHeight="1">
       <c r="A159" s="1" t="s">
         <v>95</v>
       </c>
@@ -5356,7 +5391,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:3" ht="30" customHeight="1">
       <c r="A160" s="1" t="s">
         <v>13</v>
       </c>
@@ -5367,7 +5402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:3">
       <c r="A161" s="1" t="s">
         <v>107</v>
       </c>
@@ -5378,7 +5413,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:3" ht="75" customHeight="1">
       <c r="A162" s="1" t="s">
         <v>104</v>
       </c>
@@ -5389,7 +5424,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:3">
       <c r="A163" s="1" t="s">
         <v>46</v>
       </c>
@@ -5400,7 +5435,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:3" ht="72" customHeight="1">
       <c r="A164" s="1" t="s">
         <v>377</v>
       </c>
@@ -5411,7 +5446,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:3">
       <c r="A165" s="1" t="s">
         <v>110</v>
       </c>
@@ -5422,7 +5457,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:3">
       <c r="A166" s="1" t="s">
         <v>3</v>
       </c>
@@ -5433,7 +5468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:3">
       <c r="A167" s="1" t="s">
         <v>11</v>
       </c>
@@ -5444,7 +5479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:3">
       <c r="A168" s="1" t="s">
         <v>79</v>
       </c>
@@ -5455,7 +5490,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:3" ht="30" customHeight="1">
       <c r="A169" s="1" t="s">
         <v>733</v>
       </c>
@@ -5466,7 +5501,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:3" ht="30" customHeight="1">
       <c r="A170" s="1" t="s">
         <v>736</v>
       </c>
@@ -5477,7 +5512,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:3" ht="36" customHeight="1">
       <c r="A171" s="1" t="s">
         <v>742</v>
       </c>
@@ -5488,7 +5523,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:3" ht="36" customHeight="1">
       <c r="A172" s="1" t="s">
         <v>730</v>
       </c>
@@ -5499,7 +5534,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
         <v>49</v>
       </c>
@@ -5510,7 +5545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
         <v>194</v>
       </c>
@@ -5521,7 +5556,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:3">
       <c r="A175" s="1" t="s">
         <v>161</v>
       </c>
@@ -5532,7 +5567,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:3">
       <c r="A176" s="1" t="s">
         <v>86</v>
       </c>
@@ -5543,7 +5578,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:3">
       <c r="A177" s="1" t="s">
         <v>826</v>
       </c>
@@ -5554,7 +5589,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
         <v>832</v>
       </c>
@@ -5565,7 +5600,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:3" ht="30" customHeight="1">
       <c r="A179" s="1" t="s">
         <v>802</v>
       </c>
@@ -5576,7 +5611,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
         <v>811</v>
       </c>
@@ -5587,7 +5622,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:3">
       <c r="A181" s="1" t="s">
         <v>805</v>
       </c>
@@ -5598,7 +5633,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
         <v>805</v>
       </c>
@@ -5609,7 +5644,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:3">
       <c r="A183" s="1" t="s">
         <v>182</v>
       </c>
@@ -5620,7 +5655,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:3">
       <c r="A184" s="1" t="s">
         <v>196</v>
       </c>
@@ -5631,7 +5666,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:3">
       <c r="A185" s="1" t="s">
         <v>823</v>
       </c>
@@ -5642,7 +5677,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:3">
       <c r="A186" s="1" t="s">
         <v>173</v>
       </c>
@@ -5653,7 +5688,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
         <v>312</v>
       </c>
@@ -5664,7 +5699,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:3">
       <c r="A188" s="1" t="s">
         <v>40</v>
       </c>
@@ -5675,7 +5710,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:3">
       <c r="A189" s="1" t="s">
         <v>461</v>
       </c>
@@ -5686,7 +5721,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:3" ht="30" customHeight="1">
       <c r="A190" s="1" t="s">
         <v>119</v>
       </c>
@@ -5697,7 +5732,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:3" ht="29.1" customHeight="1">
       <c r="A191" s="1" t="s">
         <v>335</v>
       </c>
@@ -5708,7 +5743,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:3">
       <c r="A192" s="1" t="s">
         <v>137</v>
       </c>
@@ -5719,7 +5754,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:3" ht="36" customHeight="1">
       <c r="A193" s="1" t="s">
         <v>5</v>
       </c>
@@ -5730,7 +5765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:3">
       <c r="A194" s="1" t="s">
         <v>76</v>
       </c>
@@ -5741,7 +5776,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:3">
       <c r="A195" s="1" t="s">
         <v>778</v>
       </c>
@@ -5752,7 +5787,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:3">
       <c r="A196" s="1" t="s">
         <v>712</v>
       </c>
@@ -5763,7 +5798,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:3">
       <c r="A197" s="1" t="s">
         <v>775</v>
       </c>
@@ -5774,7 +5809,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:3">
       <c r="A198" s="1" t="s">
         <v>793</v>
       </c>
@@ -5785,7 +5820,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:3">
       <c r="A199" s="1" t="s">
         <v>784</v>
       </c>
@@ -5796,7 +5831,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:3">
       <c r="A200" s="1" t="s">
         <v>787</v>
       </c>
@@ -5807,7 +5842,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:3">
       <c r="A201" s="1" t="s">
         <v>781</v>
       </c>
@@ -5818,7 +5853,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:3">
       <c r="A202" s="1" t="s">
         <v>193</v>
       </c>
@@ -5829,7 +5864,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:3">
       <c r="A203" s="1" t="s">
         <v>158</v>
       </c>
@@ -5840,7 +5875,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:3" ht="29.1" customHeight="1">
       <c r="A204" s="1" t="s">
         <v>315</v>
       </c>
@@ -5851,7 +5886,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:3">
       <c r="A205" s="1" t="s">
         <v>83</v>
       </c>
@@ -5862,7 +5897,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:3" ht="36" customHeight="1">
       <c r="A206" s="1" t="s">
         <v>872</v>
       </c>
@@ -5873,7 +5908,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:3">
       <c r="A207" s="1" t="s">
         <v>664</v>
       </c>
@@ -5884,7 +5919,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:3">
       <c r="A208" s="1" t="s">
         <v>859</v>
       </c>
@@ -5895,7 +5930,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:3">
       <c r="A209" s="1" t="s">
         <v>856</v>
       </c>
@@ -5906,7 +5941,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:3">
       <c r="A210" s="1" t="s">
         <v>875</v>
       </c>
@@ -5917,7 +5952,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:3">
       <c r="A211" s="1" t="s">
         <v>878</v>
       </c>
@@ -5928,7 +5963,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:3">
       <c r="A212" s="1" t="s">
         <v>853</v>
       </c>
@@ -5939,7 +5974,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:3">
       <c r="A213" s="1" t="s">
         <v>195</v>
       </c>
@@ -5950,7 +5985,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:3">
       <c r="A214" s="1" t="s">
         <v>170</v>
       </c>
@@ -5961,7 +5996,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:3">
       <c r="A215" s="1" t="s">
         <v>70</v>
       </c>
@@ -5972,7 +6007,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:3" ht="28.8">
       <c r="A216" s="1" t="s">
         <v>533</v>
       </c>
@@ -5983,7 +6018,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:3">
       <c r="A217" s="1" t="s">
         <v>548</v>
       </c>
@@ -5994,7 +6029,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:3">
       <c r="A218" s="1" t="s">
         <v>694</v>
       </c>
@@ -6005,7 +6040,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:3">
       <c r="A219" s="1" t="s">
         <v>542</v>
       </c>
@@ -6016,7 +6051,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:3">
       <c r="A220" s="1" t="s">
         <v>554</v>
       </c>
@@ -6027,7 +6062,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:3">
       <c r="A221" s="1" t="s">
         <v>536</v>
       </c>
@@ -6038,7 +6073,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:3">
       <c r="A222" s="1" t="s">
         <v>545</v>
       </c>
@@ -6049,7 +6084,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:3">
       <c r="A223" s="1" t="s">
         <v>191</v>
       </c>
@@ -6060,7 +6095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:3">
       <c r="A224" s="1" t="s">
         <v>149</v>
       </c>
@@ -6071,7 +6106,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:3">
       <c r="A225" s="1" t="s">
         <v>601</v>
       </c>
@@ -6082,7 +6117,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:3">
       <c r="A226" s="1" t="s">
         <v>604</v>
       </c>
@@ -6093,7 +6128,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:3">
       <c r="A227" s="1" t="s">
         <v>772</v>
       </c>
@@ -6104,7 +6139,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:3">
       <c r="A228" s="1" t="s">
         <v>769</v>
       </c>
@@ -6115,7 +6150,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:3" ht="30" customHeight="1">
       <c r="A229" s="1" t="s">
         <v>610</v>
       </c>
@@ -6126,7 +6161,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:3" ht="30" customHeight="1">
       <c r="A230" s="1" t="s">
         <v>232</v>
       </c>
@@ -6137,7 +6172,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:3" ht="36" customHeight="1">
       <c r="A231" s="1" t="s">
         <v>58</v>
       </c>
@@ -6148,7 +6183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:3" ht="36" customHeight="1">
       <c r="A232" s="1" t="s">
         <v>368</v>
       </c>
@@ -6159,7 +6194,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:3" ht="30" customHeight="1">
       <c r="A233" s="1" t="s">
         <v>829</v>
       </c>
@@ -6170,7 +6205,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:3">
       <c r="A234" s="1" t="s">
         <v>634</v>
       </c>
@@ -6181,7 +6216,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:3">
       <c r="A235" s="1" t="s">
         <v>616</v>
       </c>
@@ -6192,7 +6227,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:3">
       <c r="A236" s="1" t="s">
         <v>649</v>
       </c>
@@ -6203,7 +6238,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:3">
       <c r="A237" s="1" t="s">
         <v>709</v>
       </c>
@@ -6214,7 +6249,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:3" ht="45" customHeight="1">
       <c r="A238" s="1" t="s">
         <v>661</v>
       </c>
@@ -6225,7 +6260,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:3" ht="29.1" customHeight="1">
       <c r="A239" s="1" t="s">
         <v>691</v>
       </c>
@@ -6236,7 +6271,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:3" ht="36" customHeight="1">
       <c r="A240" s="1" t="s">
         <v>700</v>
       </c>
@@ -6247,7 +6282,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:3">
       <c r="A241" s="1" t="s">
         <v>718</v>
       </c>
@@ -6258,7 +6293,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:3">
       <c r="A242" s="1" t="s">
         <v>619</v>
       </c>
@@ -6269,7 +6304,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:3">
       <c r="A243" s="1" t="s">
         <v>902</v>
       </c>
@@ -6280,7 +6315,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:3">
       <c r="A244" s="1" t="s">
         <v>479</v>
       </c>
@@ -6291,7 +6326,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:3">
       <c r="A245" s="1" t="s">
         <v>905</v>
       </c>
@@ -6302,7 +6337,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:3">
       <c r="A246" s="1" t="s">
         <v>276</v>
       </c>
@@ -6313,7 +6348,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:3">
       <c r="A247" s="1" t="s">
         <v>488</v>
       </c>
@@ -6324,7 +6359,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:3">
       <c r="A248" s="1" t="s">
         <v>31</v>
       </c>
@@ -6335,7 +6370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:3">
       <c r="A249" s="1" t="s">
         <v>28</v>
       </c>
@@ -6346,7 +6381,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:3">
       <c r="A250" s="1" t="s">
         <v>464</v>
       </c>
@@ -6357,7 +6392,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:3">
       <c r="A251" s="1" t="s">
         <v>763</v>
       </c>
@@ -6368,7 +6403,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:3">
       <c r="A252" s="1" t="s">
         <v>265</v>
       </c>
@@ -6379,7 +6414,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:3">
       <c r="A253" s="1" t="s">
         <v>862</v>
       </c>
@@ -6390,7 +6425,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:3">
       <c r="A254" s="1" t="s">
         <v>383</v>
       </c>
@@ -6401,7 +6436,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:3">
       <c r="A255" s="1" t="s">
         <v>350</v>
       </c>
@@ -6412,7 +6447,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:3">
       <c r="A256" s="1" t="s">
         <v>796</v>
       </c>
@@ -6423,7 +6458,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:3">
       <c r="A257" s="1" t="s">
         <v>865</v>
       </c>
@@ -6434,7 +6469,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:3">
       <c r="A258" s="1" t="s">
         <v>557</v>
       </c>
@@ -6445,7 +6480,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:3" ht="57.6">
       <c r="A259" s="1" t="s">
         <v>326</v>
       </c>
@@ -6456,7 +6491,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:3">
       <c r="A260" s="1" t="s">
         <v>425</v>
       </c>
@@ -6467,7 +6502,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:3">
       <c r="A261" s="1" t="s">
         <v>410</v>
       </c>
@@ -6478,7 +6513,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:3">
       <c r="A262" s="1" t="s">
         <v>374</v>
       </c>
@@ -6489,7 +6524,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:3" ht="29.1" customHeight="1">
       <c r="A263" s="1" t="s">
         <v>757</v>
       </c>
@@ -6500,7 +6535,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:3">
       <c r="A264" s="1" t="s">
         <v>595</v>
       </c>
@@ -6511,7 +6546,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:3" ht="36" customHeight="1">
       <c r="A265" s="1" t="s">
         <v>359</v>
       </c>
@@ -6522,7 +6557,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:3">
       <c r="A266" s="1" t="s">
         <v>485</v>
       </c>
@@ -6533,7 +6568,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="267" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:3" ht="29.1" customHeight="1">
       <c r="A267" s="1" t="s">
         <v>577</v>
       </c>
@@ -6544,7 +6579,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:3">
       <c r="A268" s="1" t="s">
         <v>817</v>
       </c>
@@ -6555,7 +6590,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:3" ht="36" customHeight="1">
       <c r="A269" s="1" t="s">
         <v>282</v>
       </c>
@@ -6566,7 +6601,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:3" ht="28.8">
       <c r="A270" s="1" t="s">
         <v>285</v>
       </c>
@@ -6577,7 +6612,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:3">
       <c r="A271" s="1" t="s">
         <v>288</v>
       </c>
@@ -6588,7 +6623,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:3" ht="28.8">
       <c r="A272" s="1" t="s">
         <v>291</v>
       </c>
@@ -6599,7 +6634,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:3">
       <c r="A273" s="1" t="s">
         <v>279</v>
       </c>
@@ -6610,7 +6645,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="274" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:3" ht="28.8">
       <c r="A274" s="1" t="s">
         <v>739</v>
       </c>
@@ -6621,7 +6656,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:3">
       <c r="A275" s="1" t="s">
         <v>790</v>
       </c>
@@ -6632,7 +6667,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:3">
       <c r="A276" s="1" t="s">
         <v>551</v>
       </c>
@@ -6643,7 +6678,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:3">
       <c r="A277" s="1" t="s">
         <v>371</v>
       </c>
@@ -6654,7 +6689,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:3">
       <c r="A278" s="1" t="s">
         <v>911</v>
       </c>
@@ -6665,7 +6700,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:3">
       <c r="A279" s="1" t="s">
         <v>917</v>
       </c>
@@ -6676,7 +6711,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:3">
       <c r="A280" s="1" t="s">
         <v>365</v>
       </c>
@@ -6687,7 +6722,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:3">
       <c r="A281" s="1" t="s">
         <v>814</v>
       </c>
@@ -6698,7 +6733,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:3">
       <c r="A282" s="1" t="s">
         <v>920</v>
       </c>
@@ -6709,7 +6744,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:3">
       <c r="A283" s="1" t="s">
         <v>506</v>
       </c>
@@ -6720,7 +6755,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:3" ht="28.8">
       <c r="A284" s="1" t="s">
         <v>303</v>
       </c>
@@ -6731,7 +6766,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:3">
       <c r="A285" s="1" t="s">
         <v>300</v>
       </c>
@@ -6742,7 +6777,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:3">
       <c r="A286" s="1" t="s">
         <v>607</v>
       </c>
@@ -6753,7 +6788,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:3">
       <c r="A287" s="1" t="s">
         <v>908</v>
       </c>
@@ -6764,7 +6799,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:3">
       <c r="A288" s="1" t="s">
         <v>92</v>
       </c>
@@ -6775,7 +6810,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:3">
       <c r="A289" s="1" t="s">
         <v>887</v>
       </c>
@@ -6786,7 +6821,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:3">
       <c r="A290" s="1" t="s">
         <v>703</v>
       </c>
@@ -6797,7 +6832,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:3">
       <c r="A291" s="1" t="s">
         <v>890</v>
       </c>
@@ -6808,7 +6843,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:3">
       <c r="A292" s="1" t="s">
         <v>923</v>
       </c>
@@ -6819,7 +6854,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:3">
       <c r="A293" s="1" t="s">
         <v>914</v>
       </c>
@@ -6830,7 +6865,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:3">
       <c r="A294" s="1" t="s">
         <v>198</v>
       </c>
@@ -6841,7 +6876,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:3">
       <c r="A295" s="1" t="s">
         <v>179</v>
       </c>
@@ -6852,7 +6887,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:3">
       <c r="A296" s="1" t="s">
         <v>362</v>
       </c>
@@ -6863,7 +6898,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="297" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:3" ht="28.8">
       <c r="A297" s="1" t="s">
         <v>294</v>
       </c>
@@ -6874,7 +6909,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:3">
       <c r="A298" s="1" t="s">
         <v>259</v>
       </c>
@@ -6885,7 +6920,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="75" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:3" ht="57.6">
       <c r="A299" s="1" t="s">
         <v>134</v>
       </c>
@@ -6896,7 +6931,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:3" ht="43.2">
       <c r="A300" s="1" t="s">
         <v>128</v>
       </c>
@@ -6907,7 +6942,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:3" ht="29.1" customHeight="1">
       <c r="A301" s="1" t="s">
         <v>844</v>
       </c>
@@ -6918,7 +6953,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:3">
       <c r="A302" s="1" t="s">
         <v>271</v>
       </c>
@@ -6929,7 +6964,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:3" ht="36" customHeight="1">
       <c r="A303" s="1" t="s">
         <v>309</v>
       </c>
@@ -6940,7 +6975,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:3">
       <c r="A304" s="1" t="s">
         <v>274</v>
       </c>
@@ -6951,7 +6986,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:3">
       <c r="A305" s="1" t="s">
         <v>229</v>
       </c>
@@ -6962,7 +6997,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:3">
       <c r="A306" s="1" t="s">
         <v>949</v>
       </c>
@@ -6973,7 +7008,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:3">
       <c r="A307" s="1" t="s">
         <v>244</v>
       </c>
@@ -6984,7 +7019,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="308" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:3" ht="54">
       <c r="A308" s="1" t="s">
         <v>881</v>
       </c>
@@ -6995,7 +7030,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:3">
       <c r="A309" s="1" t="s">
         <v>238</v>
       </c>
@@ -7006,7 +7041,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:3">
       <c r="A310" s="1" t="s">
         <v>122</v>
       </c>
@@ -7017,7 +7052,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:3">
       <c r="A311" s="1" t="s">
         <v>55</v>
       </c>
@@ -7028,7 +7063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:3">
       <c r="A312" s="1" t="s">
         <v>946</v>
       </c>
@@ -7039,7 +7074,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:3">
       <c r="A313" s="1" t="s">
         <v>64</v>
       </c>
@@ -7050,7 +7085,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:3">
       <c r="A314" s="1" t="s">
         <v>625</v>
       </c>
@@ -7061,7 +7096,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="315" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:3" ht="28.8">
       <c r="A315" s="1" t="s">
         <v>667</v>
       </c>
@@ -7072,7 +7107,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:3">
       <c r="A316" s="1" t="s">
         <v>332</v>
       </c>
@@ -7083,7 +7118,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:3">
       <c r="A317" s="1" t="s">
         <v>329</v>
       </c>
@@ -7094,7 +7129,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="318" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="318" spans="1:3" ht="36" customHeight="1">
       <c r="A318" s="1" t="s">
         <v>524</v>
       </c>
@@ -7105,7 +7140,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:3">
       <c r="A319" s="1" t="s">
         <v>19</v>
       </c>
@@ -7116,7 +7151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:3">
       <c r="A320" s="1" t="s">
         <v>721</v>
       </c>
@@ -7127,7 +7162,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="321" spans="1:3">
       <c r="A321" s="1" t="s">
         <v>476</v>
       </c>
@@ -7138,7 +7173,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="322" spans="1:3">
       <c r="A322" s="1" t="s">
         <v>518</v>
       </c>
@@ -7149,7 +7184,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="323" spans="1:3">
       <c r="A323" s="1" t="s">
         <v>527</v>
       </c>
@@ -7160,7 +7195,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:3">
       <c r="A324" s="1" t="s">
         <v>37</v>
       </c>
@@ -7171,7 +7206,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="325" spans="1:3">
       <c r="A325" s="1" t="s">
         <v>503</v>
       </c>
@@ -7182,7 +7217,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="326" spans="1:3">
       <c r="A326" s="1" t="s">
         <v>482</v>
       </c>
@@ -7193,7 +7228,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="327" spans="1:3">
       <c r="A327" s="1" t="s">
         <v>116</v>
       </c>
@@ -7204,7 +7239,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="328" spans="1:3">
       <c r="A328" s="1" t="s">
         <v>189</v>
       </c>
@@ -7215,7 +7250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="329" spans="1:3">
       <c r="A329" s="1" t="s">
         <v>509</v>
       </c>
@@ -7226,7 +7261,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="330" spans="1:3">
       <c r="A330" s="1" t="s">
         <v>146</v>
       </c>
@@ -7237,7 +7272,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:3">
       <c r="A331" s="1" t="s">
         <v>8</v>
       </c>
@@ -7248,7 +7283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="332" spans="1:3">
       <c r="A332" s="1" t="s">
         <v>353</v>
       </c>
@@ -7259,7 +7294,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="333" spans="1:3">
       <c r="A333" s="1" t="s">
         <v>113</v>
       </c>
@@ -7270,7 +7305,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="334" spans="1:3">
       <c r="A334" s="1" t="s">
         <v>404</v>
       </c>
@@ -7281,7 +7316,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="335" spans="1:3">
       <c r="A335" s="1" t="s">
         <v>34</v>
       </c>
@@ -7292,25 +7327,46 @@
         <v>36</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B336" s="2"/>
-      <c r="C336" s="2"/>
-    </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B337" s="2"/>
-      <c r="C337" s="2"/>
-    </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B338" s="2"/>
-      <c r="C338" s="2"/>
-    </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B343" s="2"/>
-      <c r="C343" s="2"/>
-    </row>
-    <row r="344" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B344" s="2"/>
-      <c r="C344" s="2"/>
+    <row r="336" spans="1:3" ht="57.6">
+      <c r="A336" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" ht="57.6">
+      <c r="A337" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3">
+      <c r="B341" s="2"/>
+      <c r="C341" s="2"/>
+    </row>
+    <row r="342" spans="1:3">
+      <c r="B342" s="2"/>
+      <c r="C342" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added Robot Account handling for User Edit; Handled invalid properties for Robot Accounts; Updated documentation
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/andra_dregan_uipath_com/Documents/Documents/UiPath/OrchestratorManager/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/andra_dregan_uipath_com/Documents/Desktop/sr/OrchestratorManager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{914D9034-57E2-43E7-B5D3-4F57AC8B2460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E7E793E-ED53-44BF-B658-9C799E644351}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{914D9034-57E2-43E7-B5D3-4F57AC8B2460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66F3BE7A-7138-4836-875E-54F0C4ADE070}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3732" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="988">
   <si>
     <t>Name</t>
   </si>
@@ -3281,6 +3281,30 @@
   </si>
   <si>
     <t>一意のパッケージ/ライブラリバージョンが見つかりません</t>
+  </si>
+  <si>
+    <t>InvalidRobotAccountSettings</t>
+  </si>
+  <si>
+    <t>Invalid settings specified for user type Directory Robot/Robot Account.
+Robot Accounts cannot have a User Session (Allow Web Login), an Attended Robot, an Attended License or a Personal Workspace.
+Robot Accounts cannot have the Unattended Robot disabled.
+Personal details and login password are ignored for this type of user</t>
+  </si>
+  <si>
+    <t>ユーザータイプDirectoryRobotまたはロボットアカウントに無効な設定が指定されました。
+ロボットアカウントには、ユーザーセッション（Webログインを許可), Attended ロボットを,Attendedライセンス, または個人のワークスペースをを含めることはできません。
+ロボットアカウントでUnattended ロボットをを無効にすることはできません。
+このタイプのユーザーの個人情報とログインパスワードは無視されます</t>
+  </si>
+  <si>
+    <t>RobotDetailsSkipped</t>
+  </si>
+  <si>
+    <t>Successfully created, but some invalid settings were ignored. Please check the logs for more details.</t>
+  </si>
+  <si>
+    <t>正常に作成されましたが、一部の無効な設定は無視されました。認証に失敗しました。詳細はログをご確認ください。</t>
   </si>
 </sst>
 </file>
@@ -3328,10 +3352,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3631,3742 +3654,3764 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1927ABA9-1814-4487-9CEC-ABDCAF91481F}">
   <dimension ref="A1:C342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A338" sqref="A338"/>
+    <sheetView tabSelected="1" topLeftCell="A337" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A340" sqref="A340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="84.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.88671875" customWidth="1"/>
+    <col min="3" max="3" width="84.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>760</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.5" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>500</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>220</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>226</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>262</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>341</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>497</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>940</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>942</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>941</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>943</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>944</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>419</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>637</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>422</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>416</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>407</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>408</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>143</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>936</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>932</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>933</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>256</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>297</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>306</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>847</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>848</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>849</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>893</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>894</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>895</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>926</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>927</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>521</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>522</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>589</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>202</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>214</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>186</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>896</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>897</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>898</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>899</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>900</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>901</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="28.8">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>443</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>208</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>241</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>820</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>822</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="43.5" customHeight="1">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>868</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>822</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="43.5" customHeight="1">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>235</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="57.9" customHeight="1">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="54" customHeight="1">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>217</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="135" customHeight="1">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>963</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>965</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>964</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="28.8">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>413</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="90" customHeight="1">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>494</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>491</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>929</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>930</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>931</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>751</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>752</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>652</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>754</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>766</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>745</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>192</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>155</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>401</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="1" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>727</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="28.8">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>470</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="18">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="28.8">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>748</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>673</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>670</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>685</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>682</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="28.8">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>395</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="28.8">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>568</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>631</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>646</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>706</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>655</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>658</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>688</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="1" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>697</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>715</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>679</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>676</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="28.8">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>338</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>808</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>810</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>392</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="1" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>380</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="1" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>389</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="1" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>386</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="1" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>583</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="1" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>586</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="1" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>598</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>580</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="1" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>167</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>53</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>52</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>164</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>199</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="1" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>211</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>253</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>247</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="1" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>628</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="1" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="1" t="s">
+      <c r="A102" t="s">
         <v>539</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="28.8">
-      <c r="A103" s="1" t="s">
+      <c r="A103" t="s">
         <v>317</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="1" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="28.8">
-      <c r="A104" s="1" t="s">
+      <c r="A104" t="s">
         <v>323</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="1" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="28.8">
-      <c r="A105" s="1" t="s">
+      <c r="A105" t="s">
         <v>320</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="1" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="1" t="s">
+      <c r="A106" t="s">
         <v>344</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="1" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="45" customHeight="1">
-      <c r="A107" s="1" t="s">
+      <c r="A107" t="s">
         <v>131</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="45" customHeight="1">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>960</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="1" t="s">
         <v>962</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="45" customHeight="1">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>452</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="1" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>455</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="1" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="36" customHeight="1">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>530</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="1" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="36" customHeight="1">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>437</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="1" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>440</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="1" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="28.8">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>431</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="1" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="36" customHeight="1">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>643</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="1" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="28.8">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
         <v>640</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="1" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="28.8">
-      <c r="A117" s="1" t="s">
+      <c r="A117" t="s">
         <v>473</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="1" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="30" customHeight="1">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>613</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="1" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>428</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="1" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>434</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="1" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="43.5" customHeight="1">
-      <c r="A121" s="1" t="s">
+      <c r="A121" t="s">
         <v>398</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="1" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="30" customHeight="1">
-      <c r="A122" s="1" t="s">
+      <c r="A122" t="s">
         <v>515</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="1" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="54" customHeight="1">
-      <c r="A123" s="1" t="s">
+      <c r="A123" t="s">
         <v>446</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="1" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="57.6">
-      <c r="A124" s="1" t="s">
+      <c r="A124" t="s">
         <v>449</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="1" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A125" s="1" t="s">
+      <c r="A125" t="s">
         <v>835</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="1" t="s">
         <v>837</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="28.8">
-      <c r="A126" s="1" t="s">
+      <c r="A126" t="s">
         <v>841</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="1" t="s">
         <v>843</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="36" customHeight="1">
-      <c r="A127" s="1" t="s">
+      <c r="A127" t="s">
         <v>838</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="1" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="1" t="s">
+      <c r="A128" t="s">
         <v>970</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="1" t="s">
         <v>971</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="1" t="s">
         <v>972</v>
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="1" t="s">
+      <c r="A129" t="s">
         <v>967</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="1" t="s">
         <v>968</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="1" t="s">
         <v>969</v>
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="1" t="s">
+      <c r="A130" t="s">
         <v>356</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="1" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="1" t="s">
+      <c r="A131" t="s">
         <v>197</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="1" t="s">
+      <c r="A132" t="s">
         <v>176</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="1" t="s">
+      <c r="A133" t="s">
         <v>89</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="1" t="s">
+      <c r="A134" t="s">
         <v>957</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="1" t="s">
         <v>959</v>
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="1" t="s">
+      <c r="A135" t="s">
         <v>954</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="1" t="s">
         <v>955</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="1" t="s">
         <v>956</v>
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="1" t="s">
+      <c r="A136" t="s">
         <v>67</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="1" t="s">
+      <c r="A137" t="s">
         <v>563</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="1" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="1" t="s">
+      <c r="A138" t="s">
         <v>571</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="1" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="1" t="s">
+      <c r="A139" t="s">
         <v>574</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="1" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="1" t="s">
+      <c r="A140" t="s">
         <v>966</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="1" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="1" t="s">
+      <c r="A141" t="s">
         <v>190</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C141" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="1" t="s">
+      <c r="A142" t="s">
         <v>152</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A143" s="1" t="s">
+      <c r="A143" t="s">
         <v>268</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C143" s="1" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A144" s="1" t="s">
+      <c r="A144" t="s">
         <v>850</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" t="s">
         <v>851</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" t="s">
         <v>852</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A145" s="1" t="s">
+      <c r="A145" t="s">
         <v>250</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C145" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="36" customHeight="1">
-      <c r="A146" s="1" t="s">
+      <c r="A146" t="s">
         <v>467</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C146" s="1" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="36" customHeight="1">
-      <c r="A147" s="1" t="s">
+      <c r="A147" t="s">
         <v>622</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B147" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="C147" s="1" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="1" t="s">
+      <c r="A148" t="s">
         <v>799</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B148" s="1" t="s">
         <v>800</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="C148" s="1" t="s">
         <v>801</v>
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="1" t="s">
+      <c r="A149" t="s">
         <v>869</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" t="s">
         <v>870</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="C149" s="1" t="s">
         <v>871</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A150" s="1" t="s">
+      <c r="A150" t="s">
         <v>560</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B150" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C150" s="1" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" s="1" t="s">
+      <c r="A151" t="s">
         <v>884</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B151" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="C151" s="1" t="s">
         <v>886</v>
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="1" t="s">
+      <c r="A152" t="s">
         <v>724</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="C152" s="2" t="s">
+      <c r="C152" s="1" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="72">
-      <c r="A153" s="1" t="s">
+      <c r="A153" t="s">
         <v>140</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B153" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C153" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="1" t="s">
+      <c r="A154" t="s">
         <v>592</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B154" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C154" s="1" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="30" customHeight="1">
-      <c r="A155" s="1" t="s">
+      <c r="A155" t="s">
         <v>347</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B155" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C155" s="1" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="30" customHeight="1">
-      <c r="A156" s="1" t="s">
+      <c r="A156" t="s">
         <v>125</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B156" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="C156" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="30" customHeight="1">
-      <c r="A157" s="1" t="s">
+      <c r="A157" t="s">
         <v>458</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C157" s="1" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30" customHeight="1">
-      <c r="A158" s="1" t="s">
+      <c r="A158" t="s">
         <v>512</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B158" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C158" s="1" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="30" customHeight="1">
-      <c r="A159" s="1" t="s">
+      <c r="A159" t="s">
         <v>95</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B159" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C159" s="2" t="s">
+      <c r="C159" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="30" customHeight="1">
-      <c r="A160" s="1" t="s">
+      <c r="A160" t="s">
         <v>13</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B160" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C160" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" s="1" t="s">
+      <c r="A161" t="s">
         <v>107</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B161" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C161" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="75" customHeight="1">
-      <c r="A162" s="1" t="s">
+      <c r="A162" t="s">
         <v>104</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="163" spans="1:3">
-      <c r="A163" s="1" t="s">
+      <c r="A163" t="s">
         <v>46</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C163" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="72" customHeight="1">
-      <c r="A164" s="1" t="s">
+      <c r="A164" t="s">
         <v>377</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B164" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C164" s="1" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="1" t="s">
+      <c r="A165" t="s">
         <v>110</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B165" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C165" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="166" spans="1:3">
-      <c r="A166" s="1" t="s">
+      <c r="A166" t="s">
         <v>3</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B166" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C166" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" s="1" t="s">
+      <c r="A167" t="s">
         <v>11</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B167" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C167" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" s="1" t="s">
+      <c r="A168" t="s">
         <v>79</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B168" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="C168" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="30" customHeight="1">
-      <c r="A169" s="1" t="s">
+      <c r="A169" t="s">
         <v>733</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B169" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="1" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" customHeight="1">
-      <c r="A170" s="1" t="s">
+      <c r="A170" t="s">
         <v>736</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B170" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C170" s="1" t="s">
         <v>738</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="36" customHeight="1">
-      <c r="A171" s="1" t="s">
+      <c r="A171" t="s">
         <v>742</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B171" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="1" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="36" customHeight="1">
-      <c r="A172" s="1" t="s">
+      <c r="A172" t="s">
         <v>730</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C172" s="1" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173" s="1" t="s">
+      <c r="A173" t="s">
         <v>49</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C173" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="1" t="s">
+      <c r="A174" t="s">
         <v>194</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B174" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C174" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="175" spans="1:3">
-      <c r="A175" s="1" t="s">
+      <c r="A175" t="s">
         <v>161</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C175" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" s="1" t="s">
+      <c r="A176" t="s">
         <v>86</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B176" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C176" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="1" t="s">
+      <c r="A177" t="s">
         <v>826</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B177" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C177" s="1" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="1" t="s">
+      <c r="A178" t="s">
         <v>832</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B178" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="C178" s="1" t="s">
         <v>834</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="30" customHeight="1">
-      <c r="A179" s="1" t="s">
+      <c r="A179" t="s">
         <v>802</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="C179" s="2" t="s">
+      <c r="C179" s="1" t="s">
         <v>804</v>
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" s="1" t="s">
+      <c r="A180" t="s">
         <v>811</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B180" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C180" s="1" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="181" spans="1:3">
-      <c r="A181" s="1" t="s">
+      <c r="A181" t="s">
         <v>805</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B181" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C181" s="1" t="s">
         <v>952</v>
       </c>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182" s="1" t="s">
+      <c r="A182" t="s">
         <v>805</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B182" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C182" s="1" t="s">
         <v>807</v>
       </c>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183" s="1" t="s">
+      <c r="A183" t="s">
         <v>182</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C183" s="2" t="s">
+      <c r="C183" s="1" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="184" spans="1:3">
-      <c r="A184" s="1" t="s">
+      <c r="A184" t="s">
         <v>196</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="185" spans="1:3">
-      <c r="A185" s="1" t="s">
+      <c r="A185" t="s">
         <v>823</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="C185" s="2" t="s">
+      <c r="C185" s="1" t="s">
         <v>825</v>
       </c>
     </row>
     <row r="186" spans="1:3">
-      <c r="A186" s="1" t="s">
+      <c r="A186" t="s">
         <v>173</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="C186" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="187" spans="1:3">
-      <c r="A187" s="1" t="s">
+      <c r="A187" t="s">
         <v>312</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C187" s="2" t="s">
+      <c r="C187" s="1" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="188" spans="1:3">
-      <c r="A188" s="1" t="s">
+      <c r="A188" t="s">
         <v>40</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B188" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="C188" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="189" spans="1:3">
-      <c r="A189" s="1" t="s">
+      <c r="A189" t="s">
         <v>461</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="1" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="30" customHeight="1">
-      <c r="A190" s="1" t="s">
+      <c r="A190" t="s">
         <v>119</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B190" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C190" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A191" s="1" t="s">
+      <c r="A191" t="s">
         <v>335</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="C191" s="1" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" s="1" t="s">
+      <c r="A192" t="s">
         <v>137</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B192" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C192" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="36" customHeight="1">
-      <c r="A193" s="1" t="s">
+      <c r="A193" t="s">
         <v>5</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B193" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C193" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" s="1" t="s">
+      <c r="A194" t="s">
         <v>76</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B194" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C194" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="1" t="s">
+      <c r="A195" t="s">
         <v>778</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B195" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="C195" s="1" t="s">
         <v>780</v>
       </c>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196" s="1" t="s">
+      <c r="A196" t="s">
         <v>712</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B196" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C196" s="1" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="1" t="s">
+      <c r="A197" t="s">
         <v>775</v>
       </c>
-      <c r="B197" s="2" t="s">
+      <c r="B197" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="C197" s="1" t="s">
         <v>777</v>
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="1" t="s">
+      <c r="A198" t="s">
         <v>793</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B198" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="C198" s="2" t="s">
+      <c r="C198" s="1" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="1" t="s">
+      <c r="A199" t="s">
         <v>784</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="B199" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="C199" s="2" t="s">
+      <c r="C199" s="1" t="s">
         <v>786</v>
       </c>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200" s="1" t="s">
+      <c r="A200" t="s">
         <v>787</v>
       </c>
-      <c r="B200" s="2" t="s">
+      <c r="B200" s="1" t="s">
         <v>788</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="C200" s="1" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="201" spans="1:3">
-      <c r="A201" s="1" t="s">
+      <c r="A201" t="s">
         <v>781</v>
       </c>
-      <c r="B201" s="2" t="s">
+      <c r="B201" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="C201" s="1" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="202" spans="1:3">
-      <c r="A202" s="1" t="s">
+      <c r="A202" t="s">
         <v>193</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="B202" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="C202" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="203" spans="1:3">
-      <c r="A203" s="1" t="s">
+      <c r="A203" t="s">
         <v>158</v>
       </c>
-      <c r="B203" s="2" t="s">
+      <c r="B203" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="C203" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A204" s="1" t="s">
+      <c r="A204" t="s">
         <v>315</v>
       </c>
-      <c r="B204" s="2" t="s">
+      <c r="B204" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="C204" s="2" t="s">
+      <c r="C204" s="1" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="205" spans="1:3">
-      <c r="A205" s="1" t="s">
+      <c r="A205" t="s">
         <v>83</v>
       </c>
-      <c r="B205" s="2" t="s">
+      <c r="B205" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C205" s="2" t="s">
+      <c r="C205" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="36" customHeight="1">
-      <c r="A206" s="1" t="s">
+      <c r="A206" t="s">
         <v>872</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="B206" t="s">
         <v>873</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="C206" s="1" t="s">
         <v>874</v>
       </c>
     </row>
     <row r="207" spans="1:3">
-      <c r="A207" s="1" t="s">
+      <c r="A207" t="s">
         <v>664</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B207" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="C207" s="2" t="s">
+      <c r="C207" s="1" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="208" spans="1:3">
-      <c r="A208" s="1" t="s">
+      <c r="A208" t="s">
         <v>859</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B208" t="s">
         <v>860</v>
       </c>
-      <c r="C208" s="1" t="s">
+      <c r="C208" t="s">
         <v>861</v>
       </c>
     </row>
     <row r="209" spans="1:3">
-      <c r="A209" s="1" t="s">
+      <c r="A209" t="s">
         <v>856</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="B209" s="1" t="s">
         <v>857</v>
       </c>
-      <c r="C209" s="2" t="s">
+      <c r="C209" s="1" t="s">
         <v>858</v>
       </c>
     </row>
     <row r="210" spans="1:3">
-      <c r="A210" s="1" t="s">
+      <c r="A210" t="s">
         <v>875</v>
       </c>
-      <c r="B210" s="2" t="s">
+      <c r="B210" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="C210" s="2" t="s">
+      <c r="C210" s="1" t="s">
         <v>877</v>
       </c>
     </row>
     <row r="211" spans="1:3">
-      <c r="A211" s="1" t="s">
+      <c r="A211" t="s">
         <v>878</v>
       </c>
-      <c r="B211" s="2" t="s">
+      <c r="B211" s="1" t="s">
         <v>879</v>
       </c>
-      <c r="C211" s="2" t="s">
+      <c r="C211" s="1" t="s">
         <v>880</v>
       </c>
     </row>
     <row r="212" spans="1:3">
-      <c r="A212" s="1" t="s">
+      <c r="A212" t="s">
         <v>853</v>
       </c>
-      <c r="B212" s="1" t="s">
+      <c r="B212" t="s">
         <v>854</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="C212" t="s">
         <v>855</v>
       </c>
     </row>
     <row r="213" spans="1:3">
-      <c r="A213" s="1" t="s">
+      <c r="A213" t="s">
         <v>195</v>
       </c>
-      <c r="B213" s="2" t="s">
+      <c r="B213" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="C213" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="214" spans="1:3">
-      <c r="A214" s="1" t="s">
+      <c r="A214" t="s">
         <v>170</v>
       </c>
-      <c r="B214" s="2" t="s">
+      <c r="B214" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C214" s="2" t="s">
+      <c r="C214" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="215" spans="1:3">
-      <c r="A215" s="1" t="s">
+      <c r="A215" t="s">
         <v>70</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="B215" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C215" s="2" t="s">
+      <c r="C215" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="28.8">
-      <c r="A216" s="1" t="s">
+      <c r="A216" t="s">
         <v>533</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B216" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C216" s="2" t="s">
+      <c r="C216" s="1" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="1" t="s">
+      <c r="A217" t="s">
         <v>548</v>
       </c>
-      <c r="B217" s="2" t="s">
+      <c r="B217" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C217" s="2" t="s">
+      <c r="C217" s="1" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="218" spans="1:3">
-      <c r="A218" s="1" t="s">
+      <c r="A218" t="s">
         <v>694</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="B218" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="C218" s="2" t="s">
+      <c r="C218" s="1" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="219" spans="1:3">
-      <c r="A219" s="1" t="s">
+      <c r="A219" t="s">
         <v>542</v>
       </c>
-      <c r="B219" s="2" t="s">
+      <c r="B219" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="C219" s="1" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="1" t="s">
+      <c r="A220" t="s">
         <v>554</v>
       </c>
-      <c r="B220" s="2" t="s">
+      <c r="B220" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C220" s="2" t="s">
+      <c r="C220" s="1" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="221" spans="1:3">
-      <c r="A221" s="1" t="s">
+      <c r="A221" t="s">
         <v>536</v>
       </c>
-      <c r="B221" s="2" t="s">
+      <c r="B221" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="C221" s="2" t="s">
+      <c r="C221" s="1" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="1" t="s">
+      <c r="A222" t="s">
         <v>545</v>
       </c>
-      <c r="B222" s="2" t="s">
+      <c r="B222" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="C222" s="1" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="223" spans="1:3">
-      <c r="A223" s="1" t="s">
+      <c r="A223" t="s">
         <v>191</v>
       </c>
-      <c r="B223" s="2" t="s">
+      <c r="B223" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C223" s="2" t="s">
+      <c r="C223" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="224" spans="1:3">
-      <c r="A224" s="1" t="s">
+      <c r="A224" t="s">
         <v>149</v>
       </c>
-      <c r="B224" s="2" t="s">
+      <c r="B224" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="C224" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="225" spans="1:3">
-      <c r="A225" s="1" t="s">
+      <c r="A225" t="s">
         <v>601</v>
       </c>
-      <c r="B225" s="2" t="s">
+      <c r="B225" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="C225" s="2" t="s">
+      <c r="C225" s="1" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="1" t="s">
+      <c r="A226" t="s">
         <v>604</v>
       </c>
-      <c r="B226" s="2" t="s">
+      <c r="B226" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="C226" s="2" t="s">
+      <c r="C226" s="1" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="1" t="s">
+      <c r="A227" t="s">
         <v>772</v>
       </c>
-      <c r="B227" s="2" t="s">
+      <c r="B227" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="C227" s="2" t="s">
+      <c r="C227" s="1" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="228" spans="1:3">
-      <c r="A228" s="1" t="s">
+      <c r="A228" t="s">
         <v>769</v>
       </c>
-      <c r="B228" s="2" t="s">
+      <c r="B228" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="C228" s="1" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="30" customHeight="1">
-      <c r="A229" s="1" t="s">
+      <c r="A229" t="s">
         <v>610</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="B229" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="C229" s="2" t="s">
+      <c r="C229" s="1" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="30" customHeight="1">
-      <c r="A230" s="1" t="s">
+      <c r="A230" t="s">
         <v>232</v>
       </c>
-      <c r="B230" s="2" t="s">
+      <c r="B230" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C230" s="2" t="s">
+      <c r="C230" s="1" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="36" customHeight="1">
-      <c r="A231" s="1" t="s">
+      <c r="A231" t="s">
         <v>58</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="B231" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C231" s="2" t="s">
+      <c r="C231" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="36" customHeight="1">
-      <c r="A232" s="1" t="s">
+      <c r="A232" t="s">
         <v>368</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="B232" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="C232" s="1" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="30" customHeight="1">
-      <c r="A233" s="1" t="s">
+      <c r="A233" t="s">
         <v>829</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B233" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="C233" s="1" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="234" spans="1:3">
-      <c r="A234" s="1" t="s">
+      <c r="A234" t="s">
         <v>634</v>
       </c>
-      <c r="B234" s="2" t="s">
+      <c r="B234" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="C234" s="2" t="s">
+      <c r="C234" s="1" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="235" spans="1:3">
-      <c r="A235" s="1" t="s">
+      <c r="A235" t="s">
         <v>616</v>
       </c>
-      <c r="B235" s="2" t="s">
+      <c r="B235" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="C235" s="2" t="s">
+      <c r="C235" s="1" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="236" spans="1:3">
-      <c r="A236" s="1" t="s">
+      <c r="A236" t="s">
         <v>649</v>
       </c>
-      <c r="B236" s="2" t="s">
+      <c r="B236" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="C236" s="2" t="s">
+      <c r="C236" s="1" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="237" spans="1:3">
-      <c r="A237" s="1" t="s">
+      <c r="A237" t="s">
         <v>709</v>
       </c>
-      <c r="B237" s="2" t="s">
+      <c r="B237" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="C237" s="2" t="s">
+      <c r="C237" s="1" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="45" customHeight="1">
-      <c r="A238" s="1" t="s">
+      <c r="A238" t="s">
         <v>661</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="B238" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="C238" s="2" t="s">
+      <c r="C238" s="1" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A239" s="1" t="s">
+      <c r="A239" t="s">
         <v>691</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B239" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="C239" s="2" t="s">
+      <c r="C239" s="1" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="36" customHeight="1">
-      <c r="A240" s="1" t="s">
+      <c r="A240" t="s">
         <v>700</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="B240" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="C240" s="2" t="s">
+      <c r="C240" s="1" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="241" spans="1:3">
-      <c r="A241" s="1" t="s">
+      <c r="A241" t="s">
         <v>718</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="B241" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="C241" s="1" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="242" spans="1:3">
-      <c r="A242" s="1" t="s">
+      <c r="A242" t="s">
         <v>619</v>
       </c>
-      <c r="B242" s="2" t="s">
+      <c r="B242" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="C242" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="243" spans="1:3">
-      <c r="A243" s="1" t="s">
+      <c r="A243" t="s">
         <v>902</v>
       </c>
-      <c r="B243" s="1" t="s">
+      <c r="B243" t="s">
         <v>903</v>
       </c>
-      <c r="C243" s="1" t="s">
+      <c r="C243" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="244" spans="1:3">
-      <c r="A244" s="1" t="s">
+      <c r="A244" t="s">
         <v>479</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="B244" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C244" s="2" t="s">
+      <c r="C244" s="1" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="245" spans="1:3">
-      <c r="A245" s="1" t="s">
+      <c r="A245" t="s">
         <v>905</v>
       </c>
-      <c r="B245" s="1" t="s">
+      <c r="B245" t="s">
         <v>906</v>
       </c>
-      <c r="C245" s="1" t="s">
+      <c r="C245" t="s">
         <v>907</v>
       </c>
     </row>
     <row r="246" spans="1:3">
-      <c r="A246" s="1" t="s">
+      <c r="A246" t="s">
         <v>276</v>
       </c>
-      <c r="B246" s="2" t="s">
+      <c r="B246" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C246" s="2" t="s">
+      <c r="C246" s="1" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="247" spans="1:3">
-      <c r="A247" s="1" t="s">
+      <c r="A247" t="s">
         <v>488</v>
       </c>
-      <c r="B247" s="2" t="s">
+      <c r="B247" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="C247" s="2" t="s">
+      <c r="C247" s="1" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="248" spans="1:3">
-      <c r="A248" s="1" t="s">
+      <c r="A248" t="s">
         <v>31</v>
       </c>
-      <c r="B248" s="2" t="s">
+      <c r="B248" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C248" s="2" t="s">
+      <c r="C248" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="249" spans="1:3">
-      <c r="A249" s="1" t="s">
+      <c r="A249" t="s">
         <v>28</v>
       </c>
-      <c r="B249" s="2" t="s">
+      <c r="B249" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C249" s="2" t="s">
+      <c r="C249" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="250" spans="1:3">
-      <c r="A250" s="1" t="s">
+      <c r="A250" t="s">
         <v>464</v>
       </c>
-      <c r="B250" s="2" t="s">
+      <c r="B250" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C250" s="2" t="s">
+      <c r="C250" s="1" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="251" spans="1:3">
-      <c r="A251" s="1" t="s">
+      <c r="A251" t="s">
         <v>763</v>
       </c>
-      <c r="B251" s="2" t="s">
+      <c r="B251" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="C251" s="2" t="s">
+      <c r="C251" s="1" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="252" spans="1:3">
-      <c r="A252" s="1" t="s">
+      <c r="A252" t="s">
         <v>265</v>
       </c>
-      <c r="B252" s="2" t="s">
+      <c r="B252" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C252" s="2" t="s">
+      <c r="C252" s="1" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="253" spans="1:3">
-      <c r="A253" s="1" t="s">
+      <c r="A253" t="s">
         <v>862</v>
       </c>
-      <c r="B253" s="1" t="s">
+      <c r="B253" t="s">
         <v>863</v>
       </c>
-      <c r="C253" s="1" t="s">
+      <c r="C253" t="s">
         <v>864</v>
       </c>
     </row>
     <row r="254" spans="1:3">
-      <c r="A254" s="1" t="s">
+      <c r="A254" t="s">
         <v>383</v>
       </c>
-      <c r="B254" s="2" t="s">
+      <c r="B254" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C254" s="2" t="s">
+      <c r="C254" s="1" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="255" spans="1:3">
-      <c r="A255" s="1" t="s">
+      <c r="A255" t="s">
         <v>350</v>
       </c>
-      <c r="B255" s="2" t="s">
+      <c r="B255" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C255" s="2" t="s">
+      <c r="C255" s="1" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="256" spans="1:3">
-      <c r="A256" s="1" t="s">
+      <c r="A256" t="s">
         <v>796</v>
       </c>
-      <c r="B256" s="2" t="s">
+      <c r="B256" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C256" s="2" t="s">
+      <c r="C256" s="1" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="257" spans="1:3">
-      <c r="A257" s="1" t="s">
+      <c r="A257" t="s">
         <v>865</v>
       </c>
-      <c r="B257" s="2" t="s">
+      <c r="B257" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="C257" s="2" t="s">
+      <c r="C257" s="1" t="s">
         <v>867</v>
       </c>
     </row>
     <row r="258" spans="1:3">
-      <c r="A258" s="1" t="s">
+      <c r="A258" t="s">
         <v>557</v>
       </c>
-      <c r="B258" s="2" t="s">
+      <c r="B258" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C258" s="2" t="s">
+      <c r="C258" s="1" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="57.6">
-      <c r="A259" s="1" t="s">
+      <c r="A259" t="s">
         <v>326</v>
       </c>
-      <c r="B259" s="2" t="s">
+      <c r="B259" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C259" s="2" t="s">
+      <c r="C259" s="1" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="260" spans="1:3">
-      <c r="A260" s="1" t="s">
+      <c r="A260" t="s">
         <v>425</v>
       </c>
-      <c r="B260" s="2" t="s">
+      <c r="B260" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="C260" s="2" t="s">
+      <c r="C260" s="1" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="261" spans="1:3">
-      <c r="A261" s="1" t="s">
+      <c r="A261" t="s">
         <v>410</v>
       </c>
-      <c r="B261" s="2" t="s">
+      <c r="B261" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C261" s="2" t="s">
+      <c r="C261" s="1" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="262" spans="1:3">
-      <c r="A262" s="1" t="s">
+      <c r="A262" t="s">
         <v>374</v>
       </c>
-      <c r="B262" s="2" t="s">
+      <c r="B262" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C262" s="2" t="s">
+      <c r="C262" s="1" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A263" s="1" t="s">
+      <c r="A263" t="s">
         <v>757</v>
       </c>
-      <c r="B263" s="1" t="s">
+      <c r="B263" t="s">
         <v>758</v>
       </c>
-      <c r="C263" s="1" t="s">
+      <c r="C263" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="264" spans="1:3">
-      <c r="A264" s="1" t="s">
+      <c r="A264" t="s">
         <v>595</v>
       </c>
-      <c r="B264" s="2" t="s">
+      <c r="B264" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="C264" s="2" t="s">
+      <c r="C264" s="1" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="36" customHeight="1">
-      <c r="A265" s="1" t="s">
+      <c r="A265" t="s">
         <v>359</v>
       </c>
-      <c r="B265" s="2" t="s">
+      <c r="B265" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C265" s="2" t="s">
+      <c r="C265" s="1" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="266" spans="1:3">
-      <c r="A266" s="1" t="s">
+      <c r="A266" t="s">
         <v>485</v>
       </c>
-      <c r="B266" s="2" t="s">
+      <c r="B266" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C266" s="2" t="s">
+      <c r="C266" s="1" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A267" s="1" t="s">
+      <c r="A267" t="s">
         <v>577</v>
       </c>
-      <c r="B267" s="2" t="s">
+      <c r="B267" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="C267" s="2" t="s">
+      <c r="C267" s="1" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="268" spans="1:3">
-      <c r="A268" s="1" t="s">
+      <c r="A268" t="s">
         <v>817</v>
       </c>
-      <c r="B268" s="2" t="s">
+      <c r="B268" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="C268" s="2" t="s">
+      <c r="C268" s="1" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="36" customHeight="1">
-      <c r="A269" s="1" t="s">
+      <c r="A269" t="s">
         <v>282</v>
       </c>
-      <c r="B269" s="2" t="s">
+      <c r="B269" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C269" s="2" t="s">
+      <c r="C269" s="1" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="28.8">
-      <c r="A270" s="1" t="s">
+      <c r="A270" t="s">
         <v>285</v>
       </c>
-      <c r="B270" s="2" t="s">
+      <c r="B270" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C270" s="2" t="s">
+      <c r="C270" s="1" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="271" spans="1:3">
-      <c r="A271" s="1" t="s">
+      <c r="A271" t="s">
         <v>288</v>
       </c>
-      <c r="B271" s="2" t="s">
+      <c r="B271" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C271" s="2" t="s">
+      <c r="C271" s="1" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="28.8">
-      <c r="A272" s="1" t="s">
+      <c r="A272" t="s">
         <v>291</v>
       </c>
-      <c r="B272" s="2" t="s">
+      <c r="B272" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C272" s="2" t="s">
+      <c r="C272" s="1" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="273" spans="1:3">
-      <c r="A273" s="1" t="s">
+      <c r="A273" t="s">
         <v>279</v>
       </c>
-      <c r="B273" s="2" t="s">
+      <c r="B273" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C273" s="2" t="s">
+      <c r="C273" s="1" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="274" spans="1:3" ht="28.8">
-      <c r="A274" s="1" t="s">
+      <c r="A274" t="s">
         <v>739</v>
       </c>
-      <c r="B274" s="2" t="s">
+      <c r="B274" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="C274" s="2" t="s">
+      <c r="C274" s="1" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="275" spans="1:3">
-      <c r="A275" s="1" t="s">
+      <c r="A275" t="s">
         <v>790</v>
       </c>
-      <c r="B275" s="2" t="s">
+      <c r="B275" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="C275" s="2" t="s">
+      <c r="C275" s="1" t="s">
         <v>792</v>
       </c>
     </row>
     <row r="276" spans="1:3">
-      <c r="A276" s="1" t="s">
+      <c r="A276" t="s">
         <v>551</v>
       </c>
-      <c r="B276" s="2" t="s">
+      <c r="B276" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C276" s="2" t="s">
+      <c r="C276" s="1" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="277" spans="1:3">
-      <c r="A277" s="1" t="s">
+      <c r="A277" t="s">
         <v>371</v>
       </c>
-      <c r="B277" s="2" t="s">
+      <c r="B277" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C277" s="2" t="s">
+      <c r="C277" s="1" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="278" spans="1:3">
-      <c r="A278" s="1" t="s">
+      <c r="A278" t="s">
         <v>911</v>
       </c>
-      <c r="B278" s="1" t="s">
+      <c r="B278" t="s">
         <v>912</v>
       </c>
-      <c r="C278" s="1" t="s">
+      <c r="C278" t="s">
         <v>913</v>
       </c>
     </row>
     <row r="279" spans="1:3">
-      <c r="A279" s="1" t="s">
+      <c r="A279" t="s">
         <v>917</v>
       </c>
-      <c r="B279" s="1" t="s">
+      <c r="B279" t="s">
         <v>918</v>
       </c>
-      <c r="C279" s="1" t="s">
+      <c r="C279" t="s">
         <v>919</v>
       </c>
     </row>
     <row r="280" spans="1:3">
-      <c r="A280" s="1" t="s">
+      <c r="A280" t="s">
         <v>365</v>
       </c>
-      <c r="B280" s="2" t="s">
+      <c r="B280" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C280" s="2" t="s">
+      <c r="C280" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="281" spans="1:3">
-      <c r="A281" s="1" t="s">
+      <c r="A281" t="s">
         <v>814</v>
       </c>
-      <c r="B281" s="2" t="s">
+      <c r="B281" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="C281" s="2" t="s">
+      <c r="C281" s="1" t="s">
         <v>816</v>
       </c>
     </row>
     <row r="282" spans="1:3">
-      <c r="A282" s="1" t="s">
+      <c r="A282" t="s">
         <v>920</v>
       </c>
-      <c r="B282" s="2" t="s">
+      <c r="B282" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="C282" s="2" t="s">
+      <c r="C282" s="1" t="s">
         <v>922</v>
       </c>
     </row>
     <row r="283" spans="1:3">
-      <c r="A283" s="1" t="s">
+      <c r="A283" t="s">
         <v>506</v>
       </c>
-      <c r="B283" s="2" t="s">
+      <c r="B283" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="C283" s="2" t="s">
+      <c r="C283" s="1" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="28.8">
-      <c r="A284" s="1" t="s">
+      <c r="A284" t="s">
         <v>303</v>
       </c>
-      <c r="B284" s="2" t="s">
+      <c r="B284" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C284" s="2" t="s">
+      <c r="C284" s="1" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="285" spans="1:3">
-      <c r="A285" s="1" t="s">
+      <c r="A285" t="s">
         <v>300</v>
       </c>
-      <c r="B285" s="2" t="s">
+      <c r="B285" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C285" s="2" t="s">
+      <c r="C285" s="1" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="286" spans="1:3">
-      <c r="A286" s="1" t="s">
+      <c r="A286" t="s">
         <v>607</v>
       </c>
-      <c r="B286" s="2" t="s">
+      <c r="B286" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="C286" s="2" t="s">
+      <c r="C286" s="1" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="287" spans="1:3">
-      <c r="A287" s="1" t="s">
+      <c r="A287" t="s">
         <v>908</v>
       </c>
-      <c r="B287" s="1" t="s">
+      <c r="B287" t="s">
         <v>909</v>
       </c>
-      <c r="C287" s="1" t="s">
+      <c r="C287" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="288" spans="1:3">
-      <c r="A288" s="1" t="s">
+      <c r="A288" t="s">
         <v>92</v>
       </c>
-      <c r="B288" s="2" t="s">
+      <c r="B288" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C288" s="2" t="s">
+      <c r="C288" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="289" spans="1:3">
-      <c r="A289" s="1" t="s">
+      <c r="A289" t="s">
         <v>887</v>
       </c>
-      <c r="B289" s="2" t="s">
+      <c r="B289" s="1" t="s">
         <v>888</v>
       </c>
-      <c r="C289" s="2" t="s">
+      <c r="C289" s="1" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="290" spans="1:3">
-      <c r="A290" s="1" t="s">
+      <c r="A290" t="s">
         <v>703</v>
       </c>
-      <c r="B290" s="2" t="s">
+      <c r="B290" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="C290" s="2" t="s">
+      <c r="C290" s="1" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="291" spans="1:3">
-      <c r="A291" s="1" t="s">
+      <c r="A291" t="s">
         <v>890</v>
       </c>
-      <c r="B291" s="1" t="s">
+      <c r="B291" t="s">
         <v>891</v>
       </c>
-      <c r="C291" s="1" t="s">
+      <c r="C291" t="s">
         <v>892</v>
       </c>
     </row>
     <row r="292" spans="1:3">
-      <c r="A292" s="1" t="s">
+      <c r="A292" t="s">
         <v>923</v>
       </c>
-      <c r="B292" s="2" t="s">
+      <c r="B292" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="C292" s="2" t="s">
+      <c r="C292" s="1" t="s">
         <v>925</v>
       </c>
     </row>
     <row r="293" spans="1:3">
-      <c r="A293" s="1" t="s">
+      <c r="A293" t="s">
         <v>914</v>
       </c>
-      <c r="B293" s="1" t="s">
+      <c r="B293" t="s">
         <v>915</v>
       </c>
-      <c r="C293" s="1" t="s">
+      <c r="C293" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="294" spans="1:3">
-      <c r="A294" s="1" t="s">
+      <c r="A294" t="s">
         <v>198</v>
       </c>
-      <c r="B294" s="2" t="s">
+      <c r="B294" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C294" s="2" t="s">
+      <c r="C294" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="295" spans="1:3">
-      <c r="A295" s="1" t="s">
+      <c r="A295" t="s">
         <v>179</v>
       </c>
-      <c r="B295" s="2" t="s">
+      <c r="B295" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C295" s="2" t="s">
+      <c r="C295" s="1" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="296" spans="1:3">
-      <c r="A296" s="1" t="s">
+      <c r="A296" t="s">
         <v>362</v>
       </c>
-      <c r="B296" s="2" t="s">
+      <c r="B296" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C296" s="2" t="s">
+      <c r="C296" s="1" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="28.8">
-      <c r="A297" s="1" t="s">
+      <c r="A297" t="s">
         <v>294</v>
       </c>
-      <c r="B297" s="2" t="s">
+      <c r="B297" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C297" s="2" t="s">
+      <c r="C297" s="1" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="298" spans="1:3">
-      <c r="A298" s="1" t="s">
+      <c r="A298" t="s">
         <v>259</v>
       </c>
-      <c r="B298" s="2" t="s">
+      <c r="B298" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C298" s="2" t="s">
+      <c r="C298" s="1" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="57.6">
-      <c r="A299" s="1" t="s">
+      <c r="A299" t="s">
         <v>134</v>
       </c>
-      <c r="B299" s="2" t="s">
+      <c r="B299" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C299" s="2" t="s">
+      <c r="C299" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="43.2">
-      <c r="A300" s="1" t="s">
+      <c r="A300" t="s">
         <v>128</v>
       </c>
-      <c r="B300" s="2" t="s">
+      <c r="B300" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C300" s="2" t="s">
+      <c r="C300" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A301" s="1" t="s">
+      <c r="A301" t="s">
         <v>844</v>
       </c>
-      <c r="B301" s="1" t="s">
+      <c r="B301" t="s">
         <v>845</v>
       </c>
-      <c r="C301" s="1" t="s">
+      <c r="C301" t="s">
         <v>846</v>
       </c>
     </row>
     <row r="302" spans="1:3">
-      <c r="A302" s="1" t="s">
+      <c r="A302" t="s">
         <v>271</v>
       </c>
-      <c r="B302" s="2" t="s">
+      <c r="B302" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C302" s="2" t="s">
+      <c r="C302" s="1" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="36" customHeight="1">
-      <c r="A303" s="1" t="s">
+      <c r="A303" t="s">
         <v>309</v>
       </c>
-      <c r="B303" s="2" t="s">
+      <c r="B303" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C303" s="2" t="s">
+      <c r="C303" s="1" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="304" spans="1:3">
-      <c r="A304" s="1" t="s">
+      <c r="A304" t="s">
         <v>274</v>
       </c>
-      <c r="B304" s="2" t="s">
+      <c r="B304" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C304" s="2" t="s">
+      <c r="C304" s="1" t="s">
         <v>934</v>
       </c>
     </row>
     <row r="305" spans="1:3">
-      <c r="A305" s="1" t="s">
+      <c r="A305" t="s">
         <v>229</v>
       </c>
-      <c r="B305" s="2" t="s">
+      <c r="B305" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C305" s="2" t="s">
+      <c r="C305" s="1" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="306" spans="1:3">
-      <c r="A306" s="1" t="s">
+      <c r="A306" t="s">
         <v>949</v>
       </c>
-      <c r="B306" s="2" t="s">
+      <c r="B306" s="1" t="s">
         <v>953</v>
       </c>
-      <c r="C306" s="2" t="s">
+      <c r="C306" s="1" t="s">
         <v>950</v>
       </c>
     </row>
     <row r="307" spans="1:3">
-      <c r="A307" s="1" t="s">
+      <c r="A307" t="s">
         <v>244</v>
       </c>
-      <c r="B307" s="2" t="s">
+      <c r="B307" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C307" s="2" t="s">
+      <c r="C307" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="54">
-      <c r="A308" s="1" t="s">
+      <c r="A308" t="s">
         <v>881</v>
       </c>
-      <c r="B308" s="2" t="s">
+      <c r="B308" s="1" t="s">
         <v>882</v>
       </c>
-      <c r="C308" s="2" t="s">
+      <c r="C308" s="1" t="s">
         <v>883</v>
       </c>
     </row>
     <row r="309" spans="1:3">
-      <c r="A309" s="1" t="s">
+      <c r="A309" t="s">
         <v>238</v>
       </c>
-      <c r="B309" s="2" t="s">
+      <c r="B309" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C309" s="2" t="s">
+      <c r="C309" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="310" spans="1:3">
-      <c r="A310" s="1" t="s">
+      <c r="A310" t="s">
         <v>122</v>
       </c>
-      <c r="B310" s="1" t="s">
+      <c r="B310" t="s">
         <v>123</v>
       </c>
-      <c r="C310" s="1" t="s">
+      <c r="C310" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="311" spans="1:3">
-      <c r="A311" s="1" t="s">
+      <c r="A311" t="s">
         <v>55</v>
       </c>
-      <c r="B311" s="2" t="s">
+      <c r="B311" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C311" s="2" t="s">
+      <c r="C311" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="312" spans="1:3">
-      <c r="A312" s="1" t="s">
+      <c r="A312" t="s">
         <v>946</v>
       </c>
-      <c r="B312" s="2" t="s">
+      <c r="B312" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="C312" s="2" t="s">
+      <c r="C312" s="1" t="s">
         <v>948</v>
       </c>
     </row>
     <row r="313" spans="1:3">
-      <c r="A313" s="1" t="s">
+      <c r="A313" t="s">
         <v>64</v>
       </c>
-      <c r="B313" s="2" t="s">
+      <c r="B313" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C313" s="2" t="s">
+      <c r="C313" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="314" spans="1:3">
-      <c r="A314" s="1" t="s">
+      <c r="A314" t="s">
         <v>625</v>
       </c>
-      <c r="B314" s="2" t="s">
+      <c r="B314" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="C314" s="2" t="s">
+      <c r="C314" s="1" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="28.8">
-      <c r="A315" s="1" t="s">
+      <c r="A315" t="s">
         <v>667</v>
       </c>
-      <c r="B315" s="2" t="s">
+      <c r="B315" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="C315" s="2" t="s">
+      <c r="C315" s="1" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="316" spans="1:3">
-      <c r="A316" s="1" t="s">
+      <c r="A316" t="s">
         <v>332</v>
       </c>
-      <c r="B316" s="2" t="s">
+      <c r="B316" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C316" s="2" t="s">
+      <c r="C316" s="1" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="317" spans="1:3">
-      <c r="A317" s="1" t="s">
+      <c r="A317" t="s">
         <v>329</v>
       </c>
-      <c r="B317" s="2" t="s">
+      <c r="B317" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C317" s="2" t="s">
+      <c r="C317" s="1" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="36" customHeight="1">
-      <c r="A318" s="1" t="s">
+      <c r="A318" t="s">
         <v>524</v>
       </c>
-      <c r="B318" s="1" t="s">
+      <c r="B318" t="s">
         <v>525</v>
       </c>
-      <c r="C318" s="2" t="s">
+      <c r="C318" s="1" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="319" spans="1:3">
-      <c r="A319" s="1" t="s">
+      <c r="A319" t="s">
         <v>19</v>
       </c>
-      <c r="B319" s="2" t="s">
+      <c r="B319" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C319" s="2" t="s">
+      <c r="C319" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="320" spans="1:3">
-      <c r="A320" s="1" t="s">
+      <c r="A320" t="s">
         <v>721</v>
       </c>
-      <c r="B320" s="2" t="s">
+      <c r="B320" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="C320" s="2" t="s">
+      <c r="C320" s="1" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="321" spans="1:3">
-      <c r="A321" s="1" t="s">
+      <c r="A321" t="s">
         <v>476</v>
       </c>
-      <c r="B321" s="2" t="s">
+      <c r="B321" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="C321" s="2" t="s">
+      <c r="C321" s="1" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="322" spans="1:3">
-      <c r="A322" s="1" t="s">
+      <c r="A322" t="s">
         <v>518</v>
       </c>
-      <c r="B322" s="2" t="s">
+      <c r="B322" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="C322" s="2" t="s">
+      <c r="C322" s="1" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="323" spans="1:3">
-      <c r="A323" s="1" t="s">
+      <c r="A323" t="s">
         <v>527</v>
       </c>
-      <c r="B323" s="1" t="s">
+      <c r="B323" t="s">
         <v>528</v>
       </c>
-      <c r="C323" s="2" t="s">
+      <c r="C323" s="1" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="324" spans="1:3">
-      <c r="A324" s="1" t="s">
+      <c r="A324" t="s">
         <v>37</v>
       </c>
-      <c r="B324" s="2" t="s">
+      <c r="B324" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C324" s="2" t="s">
+      <c r="C324" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="325" spans="1:3">
-      <c r="A325" s="1" t="s">
+      <c r="A325" t="s">
         <v>503</v>
       </c>
-      <c r="B325" s="2" t="s">
+      <c r="B325" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="C325" s="2" t="s">
+      <c r="C325" s="1" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="326" spans="1:3">
-      <c r="A326" s="1" t="s">
+      <c r="A326" t="s">
         <v>482</v>
       </c>
-      <c r="B326" s="2" t="s">
+      <c r="B326" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="C326" s="2" t="s">
+      <c r="C326" s="1" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="327" spans="1:3">
-      <c r="A327" s="1" t="s">
+      <c r="A327" t="s">
         <v>116</v>
       </c>
-      <c r="B327" s="2" t="s">
+      <c r="B327" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C327" s="2" t="s">
+      <c r="C327" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="328" spans="1:3">
-      <c r="A328" s="1" t="s">
+      <c r="A328" t="s">
         <v>189</v>
       </c>
-      <c r="B328" s="2" t="s">
+      <c r="B328" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C328" s="2" t="s">
+      <c r="C328" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="329" spans="1:3">
-      <c r="A329" s="1" t="s">
+      <c r="A329" t="s">
         <v>509</v>
       </c>
-      <c r="B329" s="2" t="s">
+      <c r="B329" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="C329" s="2" t="s">
+      <c r="C329" s="1" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="330" spans="1:3">
-      <c r="A330" s="1" t="s">
+      <c r="A330" t="s">
         <v>146</v>
       </c>
-      <c r="B330" s="2" t="s">
+      <c r="B330" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C330" s="2" t="s">
+      <c r="C330" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="331" spans="1:3">
-      <c r="A331" s="1" t="s">
+      <c r="A331" t="s">
         <v>8</v>
       </c>
-      <c r="B331" s="2" t="s">
+      <c r="B331" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C331" s="2" t="s">
+      <c r="C331" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="332" spans="1:3">
-      <c r="A332" s="1" t="s">
+      <c r="A332" t="s">
         <v>353</v>
       </c>
-      <c r="B332" s="2" t="s">
+      <c r="B332" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C332" s="2" t="s">
+      <c r="C332" s="1" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="333" spans="1:3">
-      <c r="A333" s="1" t="s">
+      <c r="A333" t="s">
         <v>113</v>
       </c>
-      <c r="B333" s="2" t="s">
+      <c r="B333" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C333" s="2" t="s">
+      <c r="C333" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="334" spans="1:3">
-      <c r="A334" s="1" t="s">
+      <c r="A334" t="s">
         <v>404</v>
       </c>
-      <c r="B334" s="2" t="s">
+      <c r="B334" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="C334" s="2" t="s">
+      <c r="C334" s="1" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="335" spans="1:3">
-      <c r="A335" s="1" t="s">
+      <c r="A335" t="s">
         <v>34</v>
       </c>
-      <c r="B335" s="2" t="s">
+      <c r="B335" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C335" s="2" t="s">
+      <c r="C335" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="336" spans="1:3" ht="57.6">
-      <c r="A336" s="1" t="s">
+      <c r="A336" t="s">
         <v>973</v>
       </c>
-      <c r="B336" s="2" t="s">
+      <c r="B336" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="C336" s="2" t="s">
+      <c r="C336" s="1" t="s">
         <v>976</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="57.6">
-      <c r="A337" s="1" t="s">
+      <c r="A337" t="s">
         <v>974</v>
       </c>
-      <c r="B337" s="2" t="s">
+      <c r="B337" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="C337" s="2" t="s">
+      <c r="C337" s="1" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="338" spans="1:3">
-      <c r="A338" s="1" t="s">
+      <c r="A338" t="s">
         <v>979</v>
       </c>
-      <c r="B338" s="1" t="s">
+      <c r="B338" t="s">
         <v>980</v>
       </c>
-      <c r="C338" s="1" t="s">
+      <c r="C338" t="s">
         <v>981</v>
       </c>
     </row>
+    <row r="339" spans="1:3" ht="86.4">
+      <c r="A339" t="s">
+        <v>982</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" ht="28.8">
+      <c r="A340" t="s">
+        <v>985</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
     <row r="341" spans="1:3">
-      <c r="B341" s="2"/>
-      <c r="C341" s="2"/>
+      <c r="B341" s="1"/>
+      <c r="C341" s="1"/>
     </row>
     <row r="342" spans="1:3">
-      <c r="B342" s="2"/>
-      <c r="C342" s="2"/>
+      <c r="B342" s="1"/>
+      <c r="C342" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>